<commit_message>
fixed: excel upload :: create all
</commit_message>
<xml_diff>
--- a/scripts/products.xlsx
+++ b/scripts/products.xlsx
@@ -79,1546 +79,1546 @@
     <t>brandName</t>
   </si>
   <si>
-    <t>845efda7-883f-4a4c-bbe8-729afdcb651e</t>
-  </si>
-  <si>
-    <t>f0837b30-a9d0-4303-b935-20f5dcbd494f</t>
-  </si>
-  <si>
-    <t>6997937f-d5ef-48e8-add8-baec2c5cf557</t>
-  </si>
-  <si>
-    <t>8046296d-c6cf-49c8-933c-158dd8b0641d</t>
-  </si>
-  <si>
-    <t>bcb5c73f-806b-4ba7-819e-feaaa7a29517</t>
-  </si>
-  <si>
-    <t>2e75df89-713d-4616-8166-83212010b85e</t>
-  </si>
-  <si>
-    <t>156437f7-d811-47c1-a1dc-761f07bd8270</t>
-  </si>
-  <si>
-    <t>0c7b27f7-37e3-4b5f-8e15-bd93ede2bf1a</t>
-  </si>
-  <si>
-    <t>cccafa94-2181-41a8-a6fb-e827511f69a6</t>
-  </si>
-  <si>
-    <t>919096ec-604b-45d0-8452-2e95cd48eee4</t>
-  </si>
-  <si>
-    <t>92ff60d7-b0fd-4e21-bbae-12bca5e3f7d0</t>
-  </si>
-  <si>
-    <t>fae12a91-7043-406e-8dc4-d1635cf94a66</t>
-  </si>
-  <si>
-    <t>7c073ab2-546b-42ec-b4ab-a420d49517d2</t>
-  </si>
-  <si>
-    <t>113bb411-4a63-4031-b6a0-067b1930fc9d</t>
-  </si>
-  <si>
-    <t>3a270bce-0aa3-444d-b78b-b846104c30cf</t>
-  </si>
-  <si>
-    <t>30c55897-e595-423e-96b7-cb8cf2411704</t>
-  </si>
-  <si>
-    <t>6a8d01f1-8750-4b6c-9f60-f7a87140b69f</t>
-  </si>
-  <si>
-    <t>a0656f8f-9e49-4eb1-9622-c1de49a0326a</t>
-  </si>
-  <si>
-    <t>5d0a651f-5f32-49ba-a448-e9cc69ba640a</t>
-  </si>
-  <si>
-    <t>790938b6-9082-45fd-9786-fff7d5251ba7</t>
-  </si>
-  <si>
-    <t>d8b016ae-716f-4551-9f80-a15ee3a92382</t>
-  </si>
-  <si>
-    <t>81394ce2-4ad6-43f7-adec-5f75c095f6bd</t>
-  </si>
-  <si>
-    <t>78fa450c-4dc6-4f1a-aeed-fd7a50d31e68</t>
-  </si>
-  <si>
-    <t>51b783a6-5117-4d8c-968d-f636ad7736ae</t>
-  </si>
-  <si>
-    <t>d3f4a461-6605-4661-975d-c520377b8b53</t>
-  </si>
-  <si>
-    <t>57c94256-870d-4b37-bad4-b6aca09ca625</t>
-  </si>
-  <si>
-    <t>79c43cc2-5e4e-47ee-a576-a899e990244a</t>
-  </si>
-  <si>
-    <t>4618a0cd-3132-4722-9ece-05b199cdc9a3</t>
-  </si>
-  <si>
-    <t>da4bc39e-7c03-409a-87e3-706104c55c46</t>
-  </si>
-  <si>
-    <t>9d41bf81-de78-4b50-b38a-55bd27cea817</t>
-  </si>
-  <si>
-    <t>36a45eec-b2bc-4852-ba60-1758fd51c2c1</t>
-  </si>
-  <si>
-    <t>9a011646-1535-4933-940e-351ceba77433</t>
-  </si>
-  <si>
-    <t>4ed72d3e-20e1-463c-824f-602f030c09fe</t>
-  </si>
-  <si>
-    <t>b95558a0-629e-4ae0-ae1f-21a7723981a6</t>
-  </si>
-  <si>
-    <t>d0c2409e-0ff4-48d4-92f7-5cdf0ec3ae1e</t>
-  </si>
-  <si>
-    <t>58075179-3c5c-4e70-8e16-f1e7fc838a86</t>
-  </si>
-  <si>
-    <t>e2489e24-9ba7-47e0-b2e5-11c3be0b3e9a</t>
-  </si>
-  <si>
-    <t>590f656c-9639-4342-a407-5f1cd446a999</t>
-  </si>
-  <si>
-    <t>ad38b04f-880b-4615-9e60-a93afead7e8d</t>
-  </si>
-  <si>
-    <t>69a058c4-8605-473a-8b9a-c9ea0e029a79</t>
-  </si>
-  <si>
-    <t>2cc8deb6-afc3-4b65-93e3-1d4e55434059</t>
-  </si>
-  <si>
-    <t>0f922632-b454-4b90-9ea7-27aa38ac7b3b</t>
-  </si>
-  <si>
-    <t>8c2eca59-9849-454e-9a70-6e3bdeed0461</t>
-  </si>
-  <si>
-    <t>2f9401c2-6504-4503-b5b2-a3265e8abbe3</t>
-  </si>
-  <si>
-    <t>9c9a33ed-74a7-4d92-a332-3834aa66f8af</t>
-  </si>
-  <si>
-    <t>1384ab67-e6de-4ed6-9115-0e25110f01eb</t>
-  </si>
-  <si>
-    <t>751dbad7-0f91-4c9e-8ac1-7888fdb76f03</t>
-  </si>
-  <si>
-    <t>204e9212-805c-4733-821b-24e795ff3bb4</t>
-  </si>
-  <si>
-    <t>73666819-b481-4a26-a336-caa5eda4eed9</t>
-  </si>
-  <si>
-    <t>41756a3f-97cc-487f-8f02-587f73311b68</t>
-  </si>
-  <si>
-    <t>87a9da69-4e9c-494d-b207-b45db5e9a6ef</t>
-  </si>
-  <si>
-    <t>14a04ec0-707b-4bb7-8ad1-03cf5e0c5937</t>
-  </si>
-  <si>
-    <t>abea418c-038a-4488-aba9-a85f6e4fd66e</t>
-  </si>
-  <si>
-    <t>adc9a9d8-74de-4778-badf-9847cfd30210</t>
-  </si>
-  <si>
-    <t>4d03240c-3265-4ce2-9e4d-276f78946924</t>
-  </si>
-  <si>
-    <t>23e05e92-a6e1-403f-ac18-2746a492657a</t>
-  </si>
-  <si>
-    <t>8b12910d-728a-49d6-8e5c-cb714d25847a</t>
-  </si>
-  <si>
-    <t>2f7b561a-6a28-403d-8d13-e0ffe33ad056</t>
-  </si>
-  <si>
-    <t>f6dccb05-2db5-4137-9ab9-d7c308b4dbed</t>
-  </si>
-  <si>
-    <t>092df914-150a-48f5-8297-24cfdc20ff1a</t>
-  </si>
-  <si>
-    <t>e1117d6c-57ac-4924-929f-05781c5c7d20</t>
-  </si>
-  <si>
-    <t>7ec0feba-2d41-401d-9943-50a900b29bb6</t>
-  </si>
-  <si>
-    <t>6b11799b-a9f2-44fa-8341-10d6f37200bf</t>
-  </si>
-  <si>
-    <t>b276f621-78ea-4120-86de-363732bf5101</t>
-  </si>
-  <si>
-    <t>6676c569-fe66-4ea1-a0d0-7d4ee9a0ec17</t>
-  </si>
-  <si>
-    <t>997d5058-f744-4f29-a3d2-037dc0b8a784</t>
-  </si>
-  <si>
-    <t>292b590a-d8f5-49ba-870e-e55d32f96882</t>
-  </si>
-  <si>
-    <t>b179594d-2f22-4125-9028-1c952d5ca8cc</t>
-  </si>
-  <si>
-    <t>c0686675-0a2a-4e82-8938-fc36acc2807a</t>
-  </si>
-  <si>
-    <t>7aabea09-9b85-4082-8d90-0b3faa6a8b34</t>
-  </si>
-  <si>
-    <t>ab50e07d-4d2c-472c-a4b3-5095f598c42d</t>
-  </si>
-  <si>
-    <t>59802790-35ea-4eee-93e4-639e0d3a3e3f</t>
-  </si>
-  <si>
-    <t>c9d4ecce-8332-4d7d-8820-3d8c1e2ff1ed</t>
-  </si>
-  <si>
-    <t>b20db668-43e8-46c8-989f-7e9fdb6c263e</t>
-  </si>
-  <si>
-    <t>714b9291-75a8-4a57-adbf-9656a68edc77</t>
-  </si>
-  <si>
-    <t>fd168b1d-6abc-4577-a682-cf46d825cc33</t>
-  </si>
-  <si>
-    <t>85263527-56c9-43cd-b720-66d25fa1f8bb</t>
-  </si>
-  <si>
-    <t>8b4c5192-911a-44a4-b247-99c26518d03e</t>
-  </si>
-  <si>
-    <t>eb6b1bfa-1d17-4d15-9c2d-d1d28a3a0254</t>
-  </si>
-  <si>
-    <t>0e0f136f-27a9-4cc7-b0ca-20bc2613c199</t>
-  </si>
-  <si>
-    <t>91615d10-ec64-45f3-aa75-2f25544bd324</t>
-  </si>
-  <si>
-    <t>f5b77ede-1d42-4e12-b4f3-2036d6779157</t>
-  </si>
-  <si>
-    <t>cc78c45b-c585-46f1-88ea-047c8ce45540</t>
-  </si>
-  <si>
-    <t>3c4bd919-3488-43e2-8964-db2a1ce518ce</t>
-  </si>
-  <si>
-    <t>71b2c9d4-5e0e-4499-be5e-c56eb557a5e2</t>
-  </si>
-  <si>
-    <t>06218fe4-f6ea-4ef0-8413-6e5b386f2c4d</t>
-  </si>
-  <si>
-    <t>946b733f-9db8-46d0-a350-23ea2f461458</t>
-  </si>
-  <si>
-    <t>0e762623-de6e-42af-ae08-ff51beea3f24</t>
-  </si>
-  <si>
-    <t>93483178-438c-4d20-8566-c14e86a1ce0f</t>
-  </si>
-  <si>
-    <t>d45ed9a0-ada5-4939-aed6-2c7914de79cb</t>
-  </si>
-  <si>
-    <t>b78be979-b720-4fa0-9fd0-7ec03df8e80c</t>
-  </si>
-  <si>
-    <t>80afd3fe-32d0-4b4a-a31d-3c807edf808b</t>
-  </si>
-  <si>
-    <t>53702993-7300-43bf-803e-25e032fbd78e</t>
-  </si>
-  <si>
-    <t>f1cfe2a3-dbbb-4b87-a955-8e9038ae7d58</t>
-  </si>
-  <si>
-    <t>1201e9eb-8f52-4d43-9dd2-c3757f887631</t>
-  </si>
-  <si>
-    <t>1c19401e-aef9-439d-8010-4f14f5260773</t>
-  </si>
-  <si>
-    <t>349451eb-56e8-4d48-8427-8841a97841a8</t>
-  </si>
-  <si>
-    <t>18fc4b82-cd71-4203-8f2f-b4ed12f083e0</t>
-  </si>
-  <si>
-    <t>e81a905c-7441-47e4-a3d3-6674abec5f0d</t>
-  </si>
-  <si>
-    <t>7b07c2db-f021-4d1a-b123-633af19d6107</t>
-  </si>
-  <si>
-    <t>981a42c4-0717-4f7f-ae24-7d69669c2bb5</t>
-  </si>
-  <si>
-    <t>919aaad6-6ac6-4927-92d1-517bba18731d</t>
-  </si>
-  <si>
-    <t>a2e554ce-b327-4a46-9d88-b94b652b44e7</t>
-  </si>
-  <si>
-    <t>be624c39-563d-44a7-8420-40071e8c372e</t>
-  </si>
-  <si>
-    <t>83280f94-ce20-4d35-b30f-f3424f582ea6</t>
-  </si>
-  <si>
-    <t>7b859893-9591-4281-9f36-f15047b48266</t>
-  </si>
-  <si>
-    <t>239a9906-8b07-418d-a5c4-098d4cec37bb</t>
-  </si>
-  <si>
-    <t>ff385887-16b0-4949-ab9b-b210654b2548</t>
-  </si>
-  <si>
-    <t>5a66b69a-3ff6-402e-b076-7a59b91689e2</t>
-  </si>
-  <si>
-    <t>ed8109bb-edbb-4e34-a67f-537af7da764e</t>
-  </si>
-  <si>
-    <t>b4cefda3-5d8d-49bf-925a-02c1090c5e93</t>
-  </si>
-  <si>
-    <t>59909257-4673-4b4d-a557-8445498a3366</t>
-  </si>
-  <si>
-    <t>66dda89c-2278-4483-8448-a07ae498101d</t>
-  </si>
-  <si>
-    <t>fabb713f-a99a-43fa-8f4e-cacd127120f0</t>
-  </si>
-  <si>
-    <t>e58cce51-8c57-4ce7-a914-b52a8f63acad</t>
-  </si>
-  <si>
-    <t>8727efbb-ddbd-403e-a2e3-e6b057fc9fbb</t>
-  </si>
-  <si>
-    <t>908470da-8b8f-4186-8a0b-bf2d6d886f8b</t>
-  </si>
-  <si>
-    <t>cb025e15-f5d9-4b54-86d4-3c1e3250496e</t>
-  </si>
-  <si>
-    <t>021c9eb7-8bca-4ece-8215-f793cdb3a12c</t>
-  </si>
-  <si>
-    <t>a056e506-315c-44db-9327-9a8b69a9539c</t>
-  </si>
-  <si>
-    <t>801f7d3d-950f-47ca-bf07-e5f0f1838534</t>
-  </si>
-  <si>
-    <t>3dfffe83-8951-483e-bae4-3984f4b589ef</t>
-  </si>
-  <si>
-    <t>f81e76c3-5ecb-4524-9cf0-c02aac569080</t>
-  </si>
-  <si>
-    <t>56a73d76-f664-4f82-afc6-19c8c017cb8c</t>
-  </si>
-  <si>
-    <t>df51487c-f57c-4bf6-b691-0a6c8294239e</t>
-  </si>
-  <si>
-    <t>3e85371a-222e-4705-935a-21081ef2fc70</t>
-  </si>
-  <si>
-    <t>0be78bec-b556-4a0b-be6d-1b062741695b</t>
-  </si>
-  <si>
-    <t>8e315b8c-f3f3-4008-b6bd-f921d01646e1</t>
-  </si>
-  <si>
-    <t>35736cd3-1e58-4f3f-a225-24735acd346a</t>
-  </si>
-  <si>
-    <t>ec09b76c-8dec-468f-989a-2ec600604283</t>
-  </si>
-  <si>
-    <t>bece1f5b-d987-40a7-8185-272f2b85a9a8</t>
-  </si>
-  <si>
-    <t>0e74f276-00f1-4eda-925f-436094ad41fe</t>
-  </si>
-  <si>
-    <t>4add7fca-3f3d-42f1-94ad-0f989c249f8b</t>
-  </si>
-  <si>
-    <t>403f256c-b6b1-4d7e-8a70-579ec21aab02</t>
-  </si>
-  <si>
-    <t>192f80c2-76e1-43fa-a70c-f4e669d852da</t>
-  </si>
-  <si>
-    <t>050d9e89-87f8-49fc-97f7-016d912af239</t>
-  </si>
-  <si>
-    <t>61ed9444-1d37-49d0-8c1d-7c5a0c6e8054</t>
-  </si>
-  <si>
-    <t>fefbab66-b59d-4557-bf42-7ec5b6c8ab15</t>
-  </si>
-  <si>
-    <t>4f2279d5-fea3-4895-a228-2f434c879a79</t>
-  </si>
-  <si>
-    <t>cb5dd8d9-48e7-43cd-8f8b-b94508496fdb</t>
-  </si>
-  <si>
-    <t>429f7f4a-dc0d-4977-a13d-ec41151e558d</t>
-  </si>
-  <si>
-    <t>67857756-9430-4d3d-8792-eb0b5632d35f</t>
-  </si>
-  <si>
-    <t>575b5ce4-787a-466a-bd53-35bc2bcedb4f</t>
-  </si>
-  <si>
-    <t>fb407f79-b5a8-4bd2-9424-c11074ebfb59</t>
-  </si>
-  <si>
-    <t>7b0fd7e2-0d8d-4d52-aa00-4ed2ff685487</t>
-  </si>
-  <si>
-    <t>ab340280-ff1c-462c-b2ff-5a1f1f0dab8e</t>
-  </si>
-  <si>
-    <t>6e42d586-cafa-4de6-88e7-e4549f73ab9c</t>
-  </si>
-  <si>
-    <t>c8e2de46-7f77-4b0c-918e-70e0696b8fcd</t>
-  </si>
-  <si>
-    <t>5c7f3b63-1d08-4e66-81b9-43e2588a404a</t>
-  </si>
-  <si>
-    <t>972b1472-d4c8-4ed5-8b52-fa9906ccbd85</t>
-  </si>
-  <si>
-    <t>7f9d6f34-9abf-46e4-8061-384b1ae7ce68</t>
-  </si>
-  <si>
-    <t>e8836357-c28d-4df3-939e-95810b876e1c</t>
-  </si>
-  <si>
-    <t>149c29c1-d698-4d70-9393-9ca435b67f53</t>
-  </si>
-  <si>
-    <t>59b0d4e5-8ca5-45b8-a991-eec0d1bb466c</t>
-  </si>
-  <si>
-    <t>e9385002-36ae-4f69-9d9a-d96cc5529483</t>
-  </si>
-  <si>
-    <t>23ee19df-6f29-4da6-9eec-f3d035373190</t>
-  </si>
-  <si>
-    <t>8ab12b4a-4d79-4b7d-b51a-5e1c3ad273db</t>
-  </si>
-  <si>
-    <t>a788e572-9da5-46aa-97ee-e92863ebefba</t>
-  </si>
-  <si>
-    <t>7a110184-344e-4865-b11b-6471f9f774ce</t>
-  </si>
-  <si>
-    <t>0cf69819-7392-4341-8fa3-0428c401e212</t>
-  </si>
-  <si>
-    <t>3caefc1c-55ce-4571-9962-f834d0ce3105</t>
-  </si>
-  <si>
-    <t>0bf60fa7-12c6-4244-a3ab-6ceae34762e4</t>
-  </si>
-  <si>
-    <t>63b498b3-2d79-4681-beb3-8c52fff81f6e</t>
-  </si>
-  <si>
-    <t>bcc34e39-ca5e-440b-adb7-226754b7d681</t>
-  </si>
-  <si>
-    <t>aac397dc-96da-493f-9816-0dfbd3ae6054</t>
-  </si>
-  <si>
-    <t>78c80585-aaa7-40d3-a069-03348ccde18b</t>
-  </si>
-  <si>
-    <t>d072176d-5e86-4149-b2b5-42cb72141c7b</t>
-  </si>
-  <si>
-    <t>0ec0ee38-d49b-43e7-8bd6-96f3b98f768b</t>
-  </si>
-  <si>
-    <t>ff3ceb06-3741-416e-aaaf-84aba1274140</t>
-  </si>
-  <si>
-    <t>205a6bda-fb2c-4669-9bc9-381ce31d77d6</t>
-  </si>
-  <si>
-    <t>67eaa86b-8fd7-431b-9927-e9ea5775b22f</t>
-  </si>
-  <si>
-    <t>b75f9d25-8bde-482c-9228-b2f8b0c74c6e</t>
-  </si>
-  <si>
-    <t>902dc4eb-5ab5-4821-a92b-8dd16789e2f5</t>
-  </si>
-  <si>
-    <t>e4e391d8-31df-48ae-8df5-df58488ca1a9</t>
-  </si>
-  <si>
-    <t>740b528e-f4e7-4a46-83de-f946473a8f1f</t>
-  </si>
-  <si>
-    <t>157013e7-2836-4262-90bd-fb3636b077f8</t>
-  </si>
-  <si>
-    <t>12849797-9a3c-4930-aad6-74f78725729f</t>
-  </si>
-  <si>
-    <t>9fa30ee3-f9d3-45ca-a62d-712afeb18726</t>
-  </si>
-  <si>
-    <t>5866bb85-0ecd-42f4-a9db-8459c163e0c9</t>
-  </si>
-  <si>
-    <t>71d1d632-e280-4b0f-9f4a-374a9f8ea805</t>
-  </si>
-  <si>
-    <t>01fb248d-65e2-434d-b22f-253b9f7462af</t>
-  </si>
-  <si>
-    <t>07022028-67ec-4936-aa0a-efb78b639d07</t>
-  </si>
-  <si>
-    <t>756effd7-939e-4577-8580-b97a6b557b06</t>
-  </si>
-  <si>
-    <t>9ef6b277-7796-4b05-9d85-a4ca2e77a618</t>
-  </si>
-  <si>
-    <t>0dae67d4-6869-4c22-9b14-c32b151c491e</t>
-  </si>
-  <si>
-    <t>085b0b6d-ab7f-48c5-92a3-5ffa0efaef9c</t>
-  </si>
-  <si>
-    <t>9c3308ff-5caa-4e0b-973c-1a6982c3747b</t>
-  </si>
-  <si>
-    <t>02c4af06-69e7-44ed-8637-74a63e72dd67</t>
-  </si>
-  <si>
-    <t>0dd3d822-3fac-4c7e-a0f8-344e0ef51b5a</t>
-  </si>
-  <si>
-    <t>1bdb5536-82f0-4717-8d40-a15cae764dd2</t>
-  </si>
-  <si>
-    <t>758ccf53-43e7-4df0-afde-e4bf6c4bc08b</t>
-  </si>
-  <si>
-    <t>b3fd8e28-3883-4723-b16d-3e0b5e3dd032</t>
-  </si>
-  <si>
-    <t>31c93937-be2a-4292-ba03-77d16ea27980</t>
-  </si>
-  <si>
-    <t>6d095c14-66fe-4360-9d82-2b35c19d2ff3</t>
-  </si>
-  <si>
-    <t>0aad5bd2-0434-4601-b633-d0ce24856409</t>
-  </si>
-  <si>
-    <t>d7492870-269c-4e3b-b5b0-d9de32cc6f9c</t>
-  </si>
-  <si>
-    <t>07ccf51d-51a7-42a2-964e-d64b7d8e1d76</t>
-  </si>
-  <si>
-    <t>9b87dc60-2c27-4d66-ae29-c7c825362307</t>
-  </si>
-  <si>
-    <t>fbaf861d-fe2e-4503-825f-49c13955093c</t>
-  </si>
-  <si>
-    <t>8107a698-082c-4242-bce2-49fea660b561</t>
-  </si>
-  <si>
-    <t>8566d5e7-4ba6-4a6d-bbc5-8949e05bdf45</t>
-  </si>
-  <si>
-    <t>97ec6ce6-7a28-472c-8a6d-8d993efd4778</t>
-  </si>
-  <si>
-    <t>4859b117-7071-4e52-bac0-f881ed7486b8</t>
-  </si>
-  <si>
-    <t>1daa31f6-3a85-4064-a41f-30b28d0c329e</t>
-  </si>
-  <si>
-    <t>d63a3be7-2f9a-4182-83ff-76d4dc7179b0</t>
-  </si>
-  <si>
-    <t>1cc99c3a-9c54-42ad-b08e-26984e571205</t>
-  </si>
-  <si>
-    <t>09ff2bbf-d872-4537-a835-ea9e7065a704</t>
-  </si>
-  <si>
-    <t>cca08dd8-1a73-4d40-b688-673fe89acd4d</t>
-  </si>
-  <si>
-    <t>75657ab5-b3fa-42e2-a0f4-b0c4ec424da7</t>
-  </si>
-  <si>
-    <t>968c3811-ef18-4d59-8642-c60c92a21e66</t>
-  </si>
-  <si>
-    <t>695edb69-a001-45be-ad02-aa91dd7b66e0</t>
-  </si>
-  <si>
-    <t>7e43c954-0710-4276-b81c-d80815218560</t>
-  </si>
-  <si>
-    <t>d7779eb6-1cf9-44b0-8ec7-0c75bd4c7e82</t>
-  </si>
-  <si>
-    <t>2cd8f264-c9ef-4f2e-a9cb-731eabe25588</t>
-  </si>
-  <si>
-    <t>659e0dab-6925-4256-911b-02225fb4bf18</t>
-  </si>
-  <si>
-    <t>698c8008-91ed-48fb-9860-b6a8d6f4a9f7</t>
-  </si>
-  <si>
-    <t>e4159eb8-8550-407c-a8e3-cc72590f575a</t>
-  </si>
-  <si>
-    <t>04dde400-0924-4ce6-8811-f68f1642e336</t>
-  </si>
-  <si>
-    <t>4993b628-0ad1-4311-bac9-86e422bd46fd</t>
-  </si>
-  <si>
-    <t>2eed3550-f0ab-455f-a324-00116a71e3a0</t>
-  </si>
-  <si>
-    <t>b97b4680-4141-4334-9274-403a558ac761</t>
-  </si>
-  <si>
-    <t>b3d62d31-e6b3-4810-8d05-6eb95a3efbce</t>
-  </si>
-  <si>
-    <t>c5c7eb07-6a8c-469a-8802-c4c031e96243</t>
-  </si>
-  <si>
-    <t>fa992763-25bb-40a8-871b-ddfad6c56177</t>
-  </si>
-  <si>
-    <t>3444d057-db9f-4c76-a10c-8390f55480b6</t>
-  </si>
-  <si>
-    <t>4b51b7ae-df1f-4835-bf8c-dad10c7b9a05</t>
-  </si>
-  <si>
-    <t>5e043bdf-50ff-466f-b1cb-316dbaff481b</t>
-  </si>
-  <si>
-    <t>ff08edcd-2898-476a-a86e-1f828cdf1236</t>
-  </si>
-  <si>
-    <t>47c0326e-f6b8-43b5-b85b-4fca0b50d1d5</t>
-  </si>
-  <si>
-    <t>d1cd1e69-be4c-4ae8-8858-e0ae53689f08</t>
-  </si>
-  <si>
-    <t>c14453e1-01f2-4598-a884-c2a599b0c92a</t>
-  </si>
-  <si>
-    <t>882e3e90-685d-4ee6-b6ac-a0c98185a2bc</t>
-  </si>
-  <si>
-    <t>4f9949d1-c66b-4e43-a43c-54f458dbef93</t>
-  </si>
-  <si>
-    <t>86ba9419-e458-4c01-867a-2ed162b50a01</t>
-  </si>
-  <si>
-    <t>80031d6e-9ffe-4112-a23f-dded40d69ea2</t>
-  </si>
-  <si>
-    <t>09f575be-eeec-4dd4-9f70-ae5b7e7419e4</t>
-  </si>
-  <si>
-    <t>2d320935-4015-41d4-8f52-6954fa903997</t>
-  </si>
-  <si>
-    <t>f506df87-2b30-49e8-bf53-e1b01c09ad19</t>
-  </si>
-  <si>
-    <t>4e91287f-1bd8-4d93-8d5e-14605afd9fa2</t>
-  </si>
-  <si>
-    <t>52b87bc3-ff6e-47da-a92b-bfc1b73d95a3</t>
-  </si>
-  <si>
-    <t>b1aadbe1-fab2-4b65-a71c-ff5b0cbe9583</t>
-  </si>
-  <si>
-    <t>16e9acc2-25ca-4438-b794-ca55ac5498bf</t>
-  </si>
-  <si>
-    <t>36dd0d90-099d-4e51-b8ba-88606818737e</t>
-  </si>
-  <si>
-    <t>12ba75c7-56a4-4a09-9c23-f7ab39b55027</t>
-  </si>
-  <si>
-    <t>d27fd1d1-9a35-4dd4-862c-c0c148e6e4d8</t>
-  </si>
-  <si>
-    <t>fa7d3445-f116-40ba-96a5-eff2ef5261db</t>
-  </si>
-  <si>
-    <t>a07b24dd-6973-4708-9017-427c67f097ee</t>
-  </si>
-  <si>
-    <t>4c6cad74-da95-4590-862a-5e21a1eaf3d2</t>
-  </si>
-  <si>
-    <t>a6ff6b35-eeac-44df-ad2f-1a2481f60b3f</t>
-  </si>
-  <si>
-    <t>80e0ec09-dd73-4223-884b-b6461a43c442</t>
-  </si>
-  <si>
-    <t>0eb787a9-6f00-40ba-9b32-8e8f3415f273</t>
-  </si>
-  <si>
-    <t>3050ca6e-8f3b-4a01-b01e-686b3b5d10bf</t>
-  </si>
-  <si>
-    <t>7f67c13b-4d8b-4ba9-be8e-395b8c994705</t>
-  </si>
-  <si>
-    <t>4a61834a-2bad-46ac-9378-63d3b3311f86</t>
-  </si>
-  <si>
-    <t>b4509c33-a5b2-4d62-8c2e-4bcbaa6245ee</t>
-  </si>
-  <si>
-    <t>4ccb4699-569b-4cc2-8492-3c84228919ea</t>
-  </si>
-  <si>
-    <t>bbd0f8e3-1ffc-4d1d-996f-531ca53f3bf6</t>
-  </si>
-  <si>
-    <t>2435ef9e-c7a7-458f-babc-4dd029fd8f20</t>
-  </si>
-  <si>
-    <t>ce79406c-5aae-4691-b044-873c7aeb798b</t>
-  </si>
-  <si>
-    <t>0a4ca5b5-c589-4386-a07b-1b72b5b08181</t>
-  </si>
-  <si>
-    <t>2f085372-5292-4d83-8e67-281eae5a09f9</t>
-  </si>
-  <si>
-    <t>12a39b7c-265e-4de0-b7a1-baac74335c35</t>
-  </si>
-  <si>
-    <t>41e4bd15-1723-43f6-ad5f-a6b67e6c96e4</t>
-  </si>
-  <si>
-    <t>63c2872c-f6f4-4e9b-b0f9-bea2182996e9</t>
-  </si>
-  <si>
-    <t>1512bd3e-e373-4a70-af8c-2e9ed1ce6cfc</t>
-  </si>
-  <si>
-    <t>1d41c228-58d5-4ffd-87db-afee88f749a3</t>
-  </si>
-  <si>
-    <t>fac74f67-865c-4408-9177-cf5c1ee83344</t>
-  </si>
-  <si>
-    <t>5b2ce941-9b75-44df-957c-3b1249f42381</t>
-  </si>
-  <si>
-    <t>ede923d8-8859-4682-8e9e-e1158307b20c</t>
-  </si>
-  <si>
-    <t>9d43a1f8-69f3-4cd0-aeb4-874b5e1cdc40</t>
-  </si>
-  <si>
-    <t>8e63aab6-84f5-4e6e-9f11-d143e74cc721</t>
-  </si>
-  <si>
-    <t>b9eedeb1-2e9d-4a9a-827e-b07cbaaa19bf</t>
-  </si>
-  <si>
-    <t>68c1968b-9a22-4de1-86ed-e9f233397d19</t>
-  </si>
-  <si>
-    <t>c5452e66-b295-4b6f-9823-de8afeac4e4c</t>
-  </si>
-  <si>
-    <t>67ad72b1-dfae-4a66-95d5-1947b5fd249a</t>
-  </si>
-  <si>
-    <t>fe8ac729-4ac7-40f4-a7ce-018e039650f0</t>
-  </si>
-  <si>
-    <t>3e03acdb-6d7a-4390-9201-5d498d9d611b</t>
-  </si>
-  <si>
-    <t>d41e24e3-59e5-44e6-addb-7cb864183a76</t>
-  </si>
-  <si>
-    <t>19acca6f-6d4b-4142-af48-2f45f99acb2f</t>
-  </si>
-  <si>
-    <t>70dfc377-dc85-40f0-9193-bd9004e0360b</t>
-  </si>
-  <si>
-    <t>f32ce142-0b23-4c48-90e5-8c58150f35a8</t>
-  </si>
-  <si>
-    <t>dd595a32-b3f6-4dbf-a052-3744dcfffcc6</t>
-  </si>
-  <si>
-    <t>2380f11c-ccb3-4b62-a73e-3e7d70878f2b</t>
-  </si>
-  <si>
-    <t>39a0a9de-93f5-4e01-8c95-c3527a1f511d</t>
-  </si>
-  <si>
-    <t>a5cf7ebd-b8ed-4182-a64a-0dfaeb6f1e3c</t>
-  </si>
-  <si>
-    <t>993ac62c-297f-4273-bc0a-ee698c7150fe</t>
-  </si>
-  <si>
-    <t>f2df35da-40f0-4038-9af3-62b86fb39b11</t>
-  </si>
-  <si>
-    <t>b2d72e0f-f3d0-4107-bece-9d7c69daa55b</t>
-  </si>
-  <si>
-    <t>3014cdc6-9850-4ee6-aca4-e4790e46af3b</t>
-  </si>
-  <si>
-    <t>45e66cbf-2caf-4afc-b7ba-69d1d7272496</t>
-  </si>
-  <si>
-    <t>0372e4f1-246a-43cb-8da5-49146854cd23</t>
-  </si>
-  <si>
-    <t>7dfe7fa2-7338-49a9-8f2a-4df5b68bd21a</t>
-  </si>
-  <si>
-    <t>90a84f9d-9411-4474-b5b1-953a8f477352</t>
-  </si>
-  <si>
-    <t>aaf9f873-0329-4204-8fe2-84f65b6525ba</t>
-  </si>
-  <si>
-    <t>355de712-c7d7-4223-8dd4-3bd3591b156d</t>
-  </si>
-  <si>
-    <t>dfcc1747-4c26-49b0-8411-8d37a6b317a4</t>
-  </si>
-  <si>
-    <t>53f37820-9f41-4819-8a38-018ab7724e51</t>
-  </si>
-  <si>
-    <t>b71cee28-18f5-433e-832e-b3a7d8ff8d1c</t>
-  </si>
-  <si>
-    <t>fda6f6e2-59ae-490f-aa5d-6c55371f6d8e</t>
-  </si>
-  <si>
-    <t>3a1b3412-5b5c-4047-a8e7-bcba0d8dbefc</t>
-  </si>
-  <si>
-    <t>369d7158-e31c-4964-ac2b-c1e6a7308b2c</t>
-  </si>
-  <si>
-    <t>12dd4f8e-112f-4b57-8fe4-fbc66e9a4f85</t>
-  </si>
-  <si>
-    <t>1e1e1332-e6a7-4904-8d04-92d19c21f073</t>
-  </si>
-  <si>
-    <t>0606bb53-25d9-4948-a7ea-8e342c4dfeeb</t>
-  </si>
-  <si>
-    <t>6350fa48-fc6a-484e-b54c-406fb3028476</t>
-  </si>
-  <si>
-    <t>665f0f54-55a2-4c69-8f0e-9c9be27b3167</t>
-  </si>
-  <si>
-    <t>31250443-39ce-43dd-b1c0-69b28966bd88</t>
-  </si>
-  <si>
-    <t>db79a92e-1535-403a-9de2-50011b42af46</t>
-  </si>
-  <si>
-    <t>8e197ea9-77e8-4a41-9e21-3f68f59622f7</t>
-  </si>
-  <si>
-    <t>a3395d59-ec72-45a9-9018-70c9aa1ceeed</t>
-  </si>
-  <si>
-    <t>f2d6ec82-7a23-43d6-b8ea-e91c9da1faba</t>
-  </si>
-  <si>
-    <t>a4efd334-c5fc-40ba-a1d0-94514dcc21da</t>
-  </si>
-  <si>
-    <t>1dba7bb0-e3ef-4541-a14d-f8f608737695</t>
-  </si>
-  <si>
-    <t>7028b4a1-c954-4d7d-8a7e-7dbf31d9613c</t>
-  </si>
-  <si>
-    <t>37a814e9-172f-4513-8a85-41b73ce08b9c</t>
-  </si>
-  <si>
-    <t>7411b81d-50c0-43b6-9486-3469c9c0c4ff</t>
-  </si>
-  <si>
-    <t>a30ef7e7-82b7-4dd5-a494-89008a9e9b9a</t>
-  </si>
-  <si>
-    <t>17a734a8-318f-4112-b780-8a9b3bc5e904</t>
-  </si>
-  <si>
-    <t>99cba8e7-8110-405f-bade-7038c3dc451b</t>
-  </si>
-  <si>
-    <t>9e20da50-bbf5-4225-8334-5606b03f5687</t>
-  </si>
-  <si>
-    <t>8773b41e-4682-469b-afe1-118fcd38b083</t>
-  </si>
-  <si>
-    <t>28ed72f5-7e8c-40c3-bd7e-66192a1a021f</t>
-  </si>
-  <si>
-    <t>bcbbe0da-05c8-48d3-a2aa-9e5323bd23ed</t>
-  </si>
-  <si>
-    <t>8eb1b07e-9a8a-4344-8d0f-baf490a60a4f</t>
-  </si>
-  <si>
-    <t>4079cd9b-9d05-471f-8709-096ee43e3086</t>
-  </si>
-  <si>
-    <t>be1a6cef-c4a1-4e72-a335-84beba008895</t>
-  </si>
-  <si>
-    <t>fc76cdd6-cc5b-4b55-afe6-0253387c9559</t>
-  </si>
-  <si>
-    <t>cc755234-9ddb-4867-bc69-6e129dd33599</t>
-  </si>
-  <si>
-    <t>49a1abaf-ff21-4dbf-ac1f-926aad53495b</t>
-  </si>
-  <si>
-    <t>9140c1b9-49ef-4cb1-81bc-d35f5473d1c9</t>
-  </si>
-  <si>
-    <t>d9afc5b5-dc08-470b-a18d-bee1cc7f303c</t>
-  </si>
-  <si>
-    <t>7d8ab841-6853-4435-8b5d-43897676af9d</t>
-  </si>
-  <si>
-    <t>50528268-4a86-4b21-85a5-35c4bdbc46aa</t>
-  </si>
-  <si>
-    <t>2acf501b-8dcf-4877-9ebf-54f2d5fd963d</t>
-  </si>
-  <si>
-    <t>1c47f8e5-377c-41d6-af77-cb9da7bb9d0b</t>
-  </si>
-  <si>
-    <t>6c96e588-4968-452a-8510-9533dd84250d</t>
-  </si>
-  <si>
-    <t>dd5e99fc-ed6b-4221-bc84-eb2e69960028</t>
-  </si>
-  <si>
-    <t>701b21a0-1bb4-491b-95b2-42d1782e7bc6</t>
-  </si>
-  <si>
-    <t>d45d1800-2c0d-4bbe-ba24-58556a8e0624</t>
-  </si>
-  <si>
-    <t>5ed4defb-7fa6-4c75-af7d-f5ffa0c4ba3d</t>
-  </si>
-  <si>
-    <t>24b8bd8a-65b9-4dc0-83fa-8395ec9d477c</t>
-  </si>
-  <si>
-    <t>ec9e2d3a-6eb8-4586-b257-02e23f362be3</t>
-  </si>
-  <si>
-    <t>8120da58-2117-4512-b623-bd92dbeb4979</t>
-  </si>
-  <si>
-    <t>e93a2a19-1f8e-4e34-b7d3-43330fbb33dc</t>
-  </si>
-  <si>
-    <t>5a083a0b-7823-4834-a91f-a3ac5456f6c9</t>
-  </si>
-  <si>
-    <t>86c687d2-1d22-4ca3-8bd8-9f745d0a7aa2</t>
-  </si>
-  <si>
-    <t>6631e2ea-68f8-421a-819c-7ff57ba8d36a</t>
-  </si>
-  <si>
-    <t>27266bcd-c6f1-4afe-b06b-9ae29e244892</t>
-  </si>
-  <si>
-    <t>8e2fbcad-375e-481e-bcf4-d4f464096017</t>
-  </si>
-  <si>
-    <t>f4d6c790-25f2-44f9-bc38-aa961d25d4d4</t>
-  </si>
-  <si>
-    <t>221e8249-480f-4490-bc1f-9df3fadada6f</t>
-  </si>
-  <si>
-    <t>9fb87fc1-6924-4616-97d9-fdef926aef49</t>
-  </si>
-  <si>
-    <t>b407656f-9b9f-4e79-9d29-6cb43cf9462c</t>
-  </si>
-  <si>
-    <t>57054bd5-df38-4939-bd98-849321dfff65</t>
-  </si>
-  <si>
-    <t>aac0900b-c7e3-4b47-bcc3-c72bb4aa151c</t>
-  </si>
-  <si>
-    <t>afd378f1-6504-416f-8e03-a33c966fcb81</t>
-  </si>
-  <si>
-    <t>441588d3-4d26-4e81-811e-aef0b4b8bf68</t>
-  </si>
-  <si>
-    <t>b14be74c-fa20-4d8c-a235-aa36b49b109b</t>
-  </si>
-  <si>
-    <t>c946bf84-2b6a-4d53-b7c3-66e18ce076cc</t>
-  </si>
-  <si>
-    <t>4844b9bf-1dfe-4979-b701-941457848308</t>
-  </si>
-  <si>
-    <t>97f78483-2d5a-48d2-9ad3-88436872f38d</t>
-  </si>
-  <si>
-    <t>328c057d-243b-4173-aacb-8404b797b4c3</t>
-  </si>
-  <si>
-    <t>cca8c16c-8544-43f9-817b-cc3a3b2a3151</t>
-  </si>
-  <si>
-    <t>9affd253-0c77-4ee1-896e-92ef07528d4b</t>
-  </si>
-  <si>
-    <t>31c01e50-3950-4217-8639-0c70e4bb727c</t>
-  </si>
-  <si>
-    <t>26318e1d-5af6-4afc-8658-2b6e3cf0c32e</t>
-  </si>
-  <si>
-    <t>b8ce8d5c-cc31-4f26-a395-21f4ba06ca7e</t>
-  </si>
-  <si>
-    <t>2bebfb99-e304-42da-91a5-5399252dc97c</t>
-  </si>
-  <si>
-    <t>48b58441-be2e-458a-8ede-e29852aac6a2</t>
-  </si>
-  <si>
-    <t>f5ab09a9-f9c0-4b9c-aae6-15eab847de6f</t>
-  </si>
-  <si>
-    <t>bfb6b225-bacf-4573-8a01-888213f590be</t>
-  </si>
-  <si>
-    <t>2f3cc2ec-e1e5-4953-a5d1-32aed7f5d816</t>
-  </si>
-  <si>
-    <t>6ff1ef1b-3b1a-4e90-be56-16219942c634</t>
-  </si>
-  <si>
-    <t>2e5fe96f-11ef-4963-94a9-2e50ce496824</t>
-  </si>
-  <si>
-    <t>2dda3be2-b853-4b02-b0d8-a4c39a9eff99</t>
-  </si>
-  <si>
-    <t>bd62f5c2-d2a6-4987-9bf8-c10876469114</t>
-  </si>
-  <si>
-    <t>80a980a3-e7a3-4858-a104-7bd9f6ab3f66</t>
-  </si>
-  <si>
-    <t>b532cfe4-c50b-43fb-8e8e-227e78e018ed</t>
-  </si>
-  <si>
-    <t>08250867-53a6-465b-b42c-7d36ce3391b2</t>
-  </si>
-  <si>
-    <t>a52042b0-0aff-4797-9dfe-7f78577a7627</t>
-  </si>
-  <si>
-    <t>b9c3b9ae-9de4-4b3c-8b5f-50a598233783</t>
-  </si>
-  <si>
-    <t>1619bb53-4dde-4d3e-ba93-17ed8988672a</t>
-  </si>
-  <si>
-    <t>7d30e450-48aa-4c0f-ae7b-cb44f248a0b7</t>
-  </si>
-  <si>
-    <t>98b92896-80c4-437e-a29a-ce9faca6826d</t>
-  </si>
-  <si>
-    <t>34291057-9fcd-498d-af40-28648e65fd39</t>
-  </si>
-  <si>
-    <t>42737120-d2b8-4106-a062-a29e92eff4e7</t>
-  </si>
-  <si>
-    <t>2c94c415-a857-4225-8553-7eaab7fdfcc0</t>
-  </si>
-  <si>
-    <t>c15f736b-b31a-426d-881a-5c86740e4b5c</t>
-  </si>
-  <si>
-    <t>40f8976d-2668-46f4-bbcf-e2ebfbc57257</t>
-  </si>
-  <si>
-    <t>0afc744e-4ed3-4a34-9265-3087e0e07e2a</t>
-  </si>
-  <si>
-    <t>1b4f71f3-7bca-44cf-94ae-3faa7f131865</t>
-  </si>
-  <si>
-    <t>bb8993fd-0aa5-4566-8fc2-db5386dbc9aa</t>
-  </si>
-  <si>
-    <t>e4909f22-ff66-47bf-9d66-f3213d3e6061</t>
-  </si>
-  <si>
-    <t>7d397419-ca4a-4c7d-8f7b-153286808ab0</t>
-  </si>
-  <si>
-    <t>27cbf6bb-43bb-4337-9d9a-35001d8451ca</t>
-  </si>
-  <si>
-    <t>4ef3446a-3d78-47ff-a1a9-5bfb006ea64f</t>
-  </si>
-  <si>
-    <t>93b43196-c919-4813-8153-5d335f340905</t>
-  </si>
-  <si>
-    <t>fdd709db-29fa-4da4-acf2-a9767ae12412</t>
-  </si>
-  <si>
-    <t>c34cefc7-cb9f-4691-8b33-d1c14e7a9e45</t>
-  </si>
-  <si>
-    <t>157e086f-913e-49c7-bf37-3ca4883f0303</t>
-  </si>
-  <si>
-    <t>d450c229-81ff-49ea-8f3c-63b3813429e5</t>
-  </si>
-  <si>
-    <t>5da83a48-f2b5-4abc-924f-369d7b6d33ab</t>
-  </si>
-  <si>
-    <t>3dacf167-154e-4cf9-a150-c1206541703b</t>
-  </si>
-  <si>
-    <t>e8d20141-57af-467f-9e24-2c77ba2b73a1</t>
-  </si>
-  <si>
-    <t>fc8d33c5-06ea-4f55-aa1d-95ce665d823c</t>
-  </si>
-  <si>
-    <t>4becca35-1cf2-4093-ba86-45343bdf6f39</t>
-  </si>
-  <si>
-    <t>98ad846d-3daa-4a37-9595-b952017de8ea</t>
-  </si>
-  <si>
-    <t>3f08c1af-9fd1-4482-96f5-1cd5734586ee</t>
-  </si>
-  <si>
-    <t>3b23798e-9668-4768-bb13-88ea21b3bcb1</t>
-  </si>
-  <si>
-    <t>d8fd80e7-d7f5-4b28-ae81-2cac54e8c4a7</t>
-  </si>
-  <si>
-    <t>9a796539-c30f-499d-9325-3a8127fecf49</t>
-  </si>
-  <si>
-    <t>248eb5d0-757f-4ff2-b717-68ad5f6634a4</t>
-  </si>
-  <si>
-    <t>35294106-cdd2-421a-b342-5c680fbca6d9</t>
-  </si>
-  <si>
-    <t>a26357c5-aeda-41eb-9680-219c2e9ca1aa</t>
-  </si>
-  <si>
-    <t>4f83f695-e48f-4552-bc35-aae0b87ce71f</t>
-  </si>
-  <si>
-    <t>5c90f23b-ae19-4d66-977f-5b15d9589ddf</t>
-  </si>
-  <si>
-    <t>8796f2c8-16f1-4b6e-95a8-20d6acbcd7a0</t>
-  </si>
-  <si>
-    <t>64432b06-ef85-4617-bf87-c6585ac5576a</t>
-  </si>
-  <si>
-    <t>49989e47-87c1-495b-8e15-5952fe1ae56a</t>
-  </si>
-  <si>
-    <t>cc8b7fde-fa1e-41ce-9ad9-9035fe32a1eb</t>
-  </si>
-  <si>
-    <t>497fcf48-f452-48a7-a607-724b5e0b3253</t>
-  </si>
-  <si>
-    <t>a5d18bb1-22ab-4cf6-a579-6295e51d543c</t>
-  </si>
-  <si>
-    <t>a49fc299-ea86-43aa-8632-7a476f29dc9a</t>
-  </si>
-  <si>
-    <t>04df059c-6dfb-44e4-9556-6dba523f47fe</t>
-  </si>
-  <si>
-    <t>e959d37d-c7b5-4bb4-841e-408f6e7eff11</t>
-  </si>
-  <si>
-    <t>5a204250-3818-42da-8ddd-468e98524d9e</t>
-  </si>
-  <si>
-    <t>f8cf99c2-ff76-4a05-83e5-2e3378375966</t>
-  </si>
-  <si>
-    <t>33bf192d-c4c0-49f1-9e2c-447855f17c71</t>
-  </si>
-  <si>
-    <t>a6d379e5-ff56-41ad-89e2-ddc15027c908</t>
-  </si>
-  <si>
-    <t>d90030f4-a400-4323-afad-cf2b2a2cd579</t>
-  </si>
-  <si>
-    <t>76897e1d-804e-46e1-a946-a49f89532da7</t>
-  </si>
-  <si>
-    <t>bef877ab-6618-497c-aca7-7ec6795ea940</t>
-  </si>
-  <si>
-    <t>17314f3a-dba4-414d-94b2-bac1f3a35877</t>
-  </si>
-  <si>
-    <t>042019c5-b463-4cd1-a8c1-735869b6272e</t>
-  </si>
-  <si>
-    <t>18a98e4a-fc84-4afb-8544-76651856f4cf</t>
-  </si>
-  <si>
-    <t>f6cc0236-0518-45fe-833c-ab66a82d6628</t>
-  </si>
-  <si>
-    <t>888cafbb-4327-42b2-b929-391e2dde1f5a</t>
-  </si>
-  <si>
-    <t>6d659c6e-f89e-4544-b67f-2cbf95f7523b</t>
-  </si>
-  <si>
-    <t>b5b2db60-3af1-4f20-87e3-41f43d9fc6ab</t>
-  </si>
-  <si>
-    <t>f044b5dc-7c11-4b32-a438-631339b05550</t>
-  </si>
-  <si>
-    <t>31460e46-7cc5-403a-9f9a-5377d8d3fa10</t>
-  </si>
-  <si>
-    <t>794f1895-f66f-4344-8696-e804739ceebe</t>
-  </si>
-  <si>
-    <t>ab319cfb-798c-42c3-8bdd-d16188668ae7</t>
-  </si>
-  <si>
-    <t>e0d669d6-8749-4a4b-a911-4a55e4ae2426</t>
-  </si>
-  <si>
-    <t>a74ed51f-aec7-4da9-8585-4c2b14bfe207</t>
-  </si>
-  <si>
-    <t>23a191f1-7f95-408d-89c7-90175f30aa31</t>
-  </si>
-  <si>
-    <t>eac40f54-3338-4c19-80fc-5c33cfda0c5d</t>
-  </si>
-  <si>
-    <t>ceaaf5e3-0781-4d69-a8fa-1f3e2ddcd5f8</t>
-  </si>
-  <si>
-    <t>43cbf339-8a33-4e07-8da2-bd3464dc13d7</t>
-  </si>
-  <si>
-    <t>07c80f0e-e982-4a0d-92ae-71462d0c2897</t>
-  </si>
-  <si>
-    <t>5b3cc511-6a6e-46b7-9c77-38763aec94e5</t>
-  </si>
-  <si>
-    <t>8eb0ab8d-7a8b-474f-ae28-c86a69b51ecf</t>
-  </si>
-  <si>
-    <t>0808b32f-ff3b-413d-9456-27bc14e760de</t>
-  </si>
-  <si>
-    <t>2a617581-7ab9-44eb-b651-dad8d969e8ef</t>
-  </si>
-  <si>
-    <t>0cd8d7f5-8004-4a5a-b7ae-8052c4fdfae4</t>
-  </si>
-  <si>
-    <t>ac946b4a-988f-4cb7-9425-84987c202d80</t>
-  </si>
-  <si>
-    <t>649ef4e8-89d1-4a26-bd78-f4077d0ff037</t>
-  </si>
-  <si>
-    <t>129ba13d-ea04-4178-96f8-72094e4cf876</t>
-  </si>
-  <si>
-    <t>7e6a29d9-2343-43a2-8352-df346f6c8c7b</t>
-  </si>
-  <si>
-    <t>5a6eaaf6-7381-4a70-ac29-cada0c52042f</t>
-  </si>
-  <si>
-    <t>8f7a10cd-eefb-4b60-a078-4529ccf93d94</t>
-  </si>
-  <si>
-    <t>9b27eba1-8c73-4b0b-8eae-8d6796823b97</t>
-  </si>
-  <si>
-    <t>ae2b1020-37ca-43f0-91f3-21d9833487f5</t>
-  </si>
-  <si>
-    <t>85e97727-ba3d-49d0-8f90-c698094756ac</t>
-  </si>
-  <si>
-    <t>4637cb7e-8dde-4b22-a261-9b4289289448</t>
-  </si>
-  <si>
-    <t>c1b0ea92-a0e8-4f57-a7d0-3e0e500991fc</t>
-  </si>
-  <si>
-    <t>3670b917-9cab-49d7-89f6-86b755b71974</t>
-  </si>
-  <si>
-    <t>88c8fbfd-725e-4405-b6ac-25b1599cb580</t>
-  </si>
-  <si>
-    <t>23c210ae-e521-4aa0-aa45-e90bec5ff4f4</t>
-  </si>
-  <si>
-    <t>7c4f6aeb-4647-4c34-a76e-5a03c0628a69</t>
-  </si>
-  <si>
-    <t>8727f4c4-eaac-4253-bdc4-ec23af18fcf7</t>
-  </si>
-  <si>
-    <t>12881579-53a5-48bf-93b1-4cdbf73c23dc</t>
-  </si>
-  <si>
-    <t>6d529479-746d-4e01-9aaa-07476fe5be8f</t>
-  </si>
-  <si>
-    <t>5f74fd73-1e7d-42aa-9d49-16d58908fceb</t>
-  </si>
-  <si>
-    <t>098d39d2-3c35-44de-9a78-a9ccead88ebd</t>
-  </si>
-  <si>
-    <t>6c792e5a-43d0-4321-b173-a53f8cbdbff6</t>
-  </si>
-  <si>
-    <t>df4d0cd3-bf0c-41b1-8ed7-946faf13dc8c</t>
-  </si>
-  <si>
-    <t>44cbb5de-b65a-4995-849b-5a2739a25aff</t>
-  </si>
-  <si>
-    <t>4a6235b7-de90-4890-8fd8-7d6863fd0d49</t>
-  </si>
-  <si>
-    <t>c9ffa9bd-4278-4b74-92b0-cf617e942103</t>
-  </si>
-  <si>
-    <t>fefffa8e-c09f-4080-8360-9e506586b623</t>
-  </si>
-  <si>
-    <t>d4f7151e-fe3c-47ab-b114-08c0774dbfe9</t>
-  </si>
-  <si>
-    <t>16a7f66b-31f9-4884-807b-42f02c991be3</t>
-  </si>
-  <si>
-    <t>673848d5-a9d5-489e-84c0-00ff9616929a</t>
-  </si>
-  <si>
-    <t>56c20d0e-6b6e-45bf-8a22-5b50e2365d0e</t>
-  </si>
-  <si>
-    <t>651d6fc1-c463-4aa7-a543-821f5c3426dd</t>
-  </si>
-  <si>
-    <t>8579c33f-1382-4872-844f-4b523a9a9a78</t>
-  </si>
-  <si>
-    <t>a235c19e-1737-41ec-b145-14c85fb5e59b</t>
-  </si>
-  <si>
-    <t>6d866754-d691-403b-b013-e5d22e7bb435</t>
-  </si>
-  <si>
-    <t>d99222bd-3cc0-4d0e-8711-8a29a3d57208</t>
-  </si>
-  <si>
-    <t>2215c1d1-e2b0-4e0b-8d99-a9a6ebec948c</t>
-  </si>
-  <si>
-    <t>3cf57226-b15d-45c0-8313-399d4f94a3a7</t>
-  </si>
-  <si>
-    <t>cc295f4c-45ab-4137-aa13-67d596c8b2fd</t>
-  </si>
-  <si>
-    <t>788d001f-dd41-47e0-995d-3fe185e37b9e</t>
-  </si>
-  <si>
-    <t>81b7eb39-2de4-4e4b-baec-49b1c3f0f325</t>
-  </si>
-  <si>
-    <t>841d0586-e768-4b80-9786-c3e38cf97ca3</t>
-  </si>
-  <si>
-    <t>4e0eb7ca-57f8-4567-a42b-be61c358c871</t>
-  </si>
-  <si>
-    <t>304aa115-6a2c-4535-b80e-4107a580baed</t>
-  </si>
-  <si>
-    <t>ac694cf3-2678-4c93-8e53-0f0a512eaba3</t>
-  </si>
-  <si>
-    <t>81ef954c-a198-45ef-8dc9-cab601d8f658</t>
-  </si>
-  <si>
-    <t>f2c26ace-febf-4cd2-be95-7d3fd1ce1dd4</t>
-  </si>
-  <si>
-    <t>ba12c334-e13d-4965-9d39-b415a98a309c</t>
-  </si>
-  <si>
-    <t>0240519d-6c8f-43f3-8a12-823ef62ea555</t>
-  </si>
-  <si>
-    <t>e69f578a-cd10-4af8-b33a-1375a25e78c2</t>
-  </si>
-  <si>
-    <t>f52582f7-880d-47dc-9125-ec772d7fc8de</t>
-  </si>
-  <si>
-    <t>17c213bb-343d-463d-80af-1175fa52e78d</t>
-  </si>
-  <si>
-    <t>7763cf46-3739-4543-99b6-ece3bd40b0b9</t>
-  </si>
-  <si>
-    <t>09c1943f-dfa2-4aeb-9f13-b3de370c0239</t>
-  </si>
-  <si>
-    <t>919a395d-bcd9-4a6a-bed8-5081c92a19c7</t>
-  </si>
-  <si>
-    <t>139078f1-6a21-4504-ba74-d630143fc294</t>
-  </si>
-  <si>
-    <t>3565f025-3df1-42bf-a83e-b79c1968f36f</t>
-  </si>
-  <si>
-    <t>b76f4625-4a13-4118-a23d-1b8f7216ae12</t>
-  </si>
-  <si>
-    <t>6460439d-6804-45bf-9f3b-2d87dc37ac80</t>
-  </si>
-  <si>
-    <t>d8bdb4f4-e07c-487c-b31b-0070a047c174</t>
+    <t>440da91f-902b-4c9a-a37f-2f81c4ec5be0</t>
+  </si>
+  <si>
+    <t>90fb3897-d334-4e7e-b7d8-a6ffd0fa3d63</t>
+  </si>
+  <si>
+    <t>789258bb-9416-44fb-9bd3-bd4bfcb995fc</t>
+  </si>
+  <si>
+    <t>fc3a23c1-95e9-4e15-a03c-866edf43d60d</t>
+  </si>
+  <si>
+    <t>3c7a212e-90a4-4469-9662-cca5d634c6f6</t>
+  </si>
+  <si>
+    <t>35b0513e-d9c2-43b0-a0f6-254eb0ead340</t>
+  </si>
+  <si>
+    <t>185e7499-3cb6-43b9-89a1-aeb5979f0d81</t>
+  </si>
+  <si>
+    <t>7dba53fc-4f9e-479b-9064-5c1a3cdd540a</t>
+  </si>
+  <si>
+    <t>242df51a-3de2-4740-951a-861fb317719b</t>
+  </si>
+  <si>
+    <t>0f79fdc6-d2f1-453d-8e9d-bb1f96d40708</t>
+  </si>
+  <si>
+    <t>5c8b3ac0-6e42-408e-aefb-a1d1e4d151de</t>
+  </si>
+  <si>
+    <t>17f78b43-27ee-4a09-9a80-ba5493b46260</t>
+  </si>
+  <si>
+    <t>137f3b2f-a28e-4f4f-bf34-152704514750</t>
+  </si>
+  <si>
+    <t>a8b9e244-2c41-45c3-a111-f0218baabee4</t>
+  </si>
+  <si>
+    <t>ef923da3-5d2d-4586-ab24-e3999380ec33</t>
+  </si>
+  <si>
+    <t>1be1b171-f610-45ed-8a63-3faf795d5ffe</t>
+  </si>
+  <si>
+    <t>39aeed87-a627-4af6-8f04-41b08a9f4f93</t>
+  </si>
+  <si>
+    <t>df78103c-21f4-4181-ad91-7099cf637264</t>
+  </si>
+  <si>
+    <t>d96ec0c3-9c22-40ff-bfb1-15e025269500</t>
+  </si>
+  <si>
+    <t>6b48d1b9-d876-4436-b0e9-26bf2289480f</t>
+  </si>
+  <si>
+    <t>2e4a972e-2292-4526-bded-ee4dd40c5c0b</t>
+  </si>
+  <si>
+    <t>ba8c5d4f-4550-43c2-9eac-76b07e6569af</t>
+  </si>
+  <si>
+    <t>9b321d9a-f9d8-4a85-87fd-698c6a8b55cd</t>
+  </si>
+  <si>
+    <t>c7de5839-b723-4c40-b590-c5fd2596d235</t>
+  </si>
+  <si>
+    <t>ae08837f-ffbb-475d-88e3-fee1ebd325f2</t>
+  </si>
+  <si>
+    <t>87febbbf-d499-4a3a-b073-0d7d607dbac4</t>
+  </si>
+  <si>
+    <t>1bc856b0-0f17-4b59-b875-eded1283c458</t>
+  </si>
+  <si>
+    <t>e632b520-c4f6-4e19-982f-92426093cbab</t>
+  </si>
+  <si>
+    <t>d70e33ab-b368-4607-bfd6-7bf70b3954c9</t>
+  </si>
+  <si>
+    <t>c3eef36d-cf35-4747-b20c-11762d1de3e2</t>
+  </si>
+  <si>
+    <t>90f56fbe-6905-4ee2-9ec9-c6049b92ddd0</t>
+  </si>
+  <si>
+    <t>870f65bf-442f-44ca-8b5f-70ed5d2a41d8</t>
+  </si>
+  <si>
+    <t>d015f609-a7bc-4ffa-8d9f-6a44535c7642</t>
+  </si>
+  <si>
+    <t>db4deef3-5c14-49f6-9375-1020c1c6d7fb</t>
+  </si>
+  <si>
+    <t>626f11f0-9019-4350-9034-6c45b1a7bbbc</t>
+  </si>
+  <si>
+    <t>4d57c788-a366-484b-90dd-6104d8485354</t>
+  </si>
+  <si>
+    <t>e4ba2c98-0c88-4d8e-9bd3-db20f5c269aa</t>
+  </si>
+  <si>
+    <t>110d7b76-6355-4d4d-8381-085de6e15959</t>
+  </si>
+  <si>
+    <t>4870414a-0afe-4a11-ad75-47f54ca5b9b2</t>
+  </si>
+  <si>
+    <t>da2007b5-13e9-43c3-8d7c-05fd08217b6d</t>
+  </si>
+  <si>
+    <t>1ce68d91-c10b-4451-adee-e2bc3053c211</t>
+  </si>
+  <si>
+    <t>fd621ff6-a544-46a9-b8ae-4edaab577467</t>
+  </si>
+  <si>
+    <t>1fa3646c-c6c8-405f-a43b-3aff1ff1bd2d</t>
+  </si>
+  <si>
+    <t>c36cb9cc-553f-4cb0-bc7a-6f0c1c06fb45</t>
+  </si>
+  <si>
+    <t>b1ce8c45-447e-4d6e-b91b-062208beef2b</t>
+  </si>
+  <si>
+    <t>ba0a0166-6a88-4ba7-b8e3-d72da95d7891</t>
+  </si>
+  <si>
+    <t>645282d8-c72f-4be8-adec-feb35914ce64</t>
+  </si>
+  <si>
+    <t>93ef4776-8bdc-46a2-9214-3a502c21253c</t>
+  </si>
+  <si>
+    <t>f5e7f196-8239-41f0-8a3d-1d3ae0981685</t>
+  </si>
+  <si>
+    <t>6a56a619-0542-40b1-9a8e-a25988e842a1</t>
+  </si>
+  <si>
+    <t>18e6dba0-ee04-4c03-ba44-a2ade75c5f1e</t>
+  </si>
+  <si>
+    <t>97ba90a3-c08e-4d89-86fd-fe0db25dfbf6</t>
+  </si>
+  <si>
+    <t>8354045e-9ef5-4e01-aa94-62c4c787407d</t>
+  </si>
+  <si>
+    <t>df375bf5-0847-4e69-88fa-246da3e99df6</t>
+  </si>
+  <si>
+    <t>ae6815bd-2134-4236-b4e8-20bb683f61c6</t>
+  </si>
+  <si>
+    <t>69844f16-b0cd-4492-a910-1d01f96cf045</t>
+  </si>
+  <si>
+    <t>2870d7c9-faa6-411a-a0a6-008d415c025f</t>
+  </si>
+  <si>
+    <t>18666133-c141-47ba-ae29-6db5718d0aef</t>
+  </si>
+  <si>
+    <t>8ede88db-bf2a-4a8c-8cb0-6a3a00da3e10</t>
+  </si>
+  <si>
+    <t>0fdd4a20-ff09-4ca6-a29e-23aa25235530</t>
+  </si>
+  <si>
+    <t>55ec2bb3-5974-4dd7-80c8-deca8994f36e</t>
+  </si>
+  <si>
+    <t>30d5438c-793f-4876-8dd6-1e6114281b16</t>
+  </si>
+  <si>
+    <t>ac7dad86-bee2-4cd5-aa20-cbc03c7471df</t>
+  </si>
+  <si>
+    <t>7da8af6f-5b49-4634-85fc-083f1c651cbb</t>
+  </si>
+  <si>
+    <t>82229e04-494c-4938-967e-8f6bc6ab3488</t>
+  </si>
+  <si>
+    <t>03aac07e-736d-4056-8cee-0d2cd96d162e</t>
+  </si>
+  <si>
+    <t>ca4f5dbe-fbef-4a7b-8517-9db0ec78e44f</t>
+  </si>
+  <si>
+    <t>9e01fc0e-c619-4d2b-982a-914c9617bdfa</t>
+  </si>
+  <si>
+    <t>913b59bf-ae30-48e7-821b-02e199a7a407</t>
+  </si>
+  <si>
+    <t>f39ac0fd-f110-46dc-86c4-c00fa7da41bd</t>
+  </si>
+  <si>
+    <t>0c97c8ca-746e-47fa-8124-2f29d9ff28f5</t>
+  </si>
+  <si>
+    <t>c59b7871-b52c-46a9-a331-49744c943b06</t>
+  </si>
+  <si>
+    <t>76f5fb6f-ecf2-4a42-95f6-afbc593fd59b</t>
+  </si>
+  <si>
+    <t>77e729f5-3b15-4d51-b357-b1fe694917ab</t>
+  </si>
+  <si>
+    <t>8b489a85-25e9-4db8-a3b1-62e14c59a006</t>
+  </si>
+  <si>
+    <t>493e1b52-3f1c-49c7-b7c1-b9dbb79f4a62</t>
+  </si>
+  <si>
+    <t>050d7cd9-30c5-46d8-9966-0f5baa92af60</t>
+  </si>
+  <si>
+    <t>c612d478-6dfa-4731-adc5-e24bd0ed1108</t>
+  </si>
+  <si>
+    <t>ea59bd5c-59fb-43a4-9432-b50011018f8b</t>
+  </si>
+  <si>
+    <t>9ca038c1-834e-4737-910b-0dbd5d0cc0a0</t>
+  </si>
+  <si>
+    <t>657a6892-34c7-493e-9d89-44d374a863c7</t>
+  </si>
+  <si>
+    <t>1857f470-012a-4d88-a804-31252e1fc89f</t>
+  </si>
+  <si>
+    <t>7a29d6b3-d014-43f0-9e3d-16f3b289426b</t>
+  </si>
+  <si>
+    <t>3a92566e-9a9f-4e66-9f33-af8b58d740ea</t>
+  </si>
+  <si>
+    <t>73ed453f-76a9-4117-9e84-d40be32f970e</t>
+  </si>
+  <si>
+    <t>a36d9d59-c0c3-4da8-9c8d-8b5266b2bc13</t>
+  </si>
+  <si>
+    <t>e395c624-8ab1-46c2-aa6f-efc74f870b2e</t>
+  </si>
+  <si>
+    <t>7269038d-1f41-4da0-9a8c-1bf641120d1c</t>
+  </si>
+  <si>
+    <t>cb051c96-350c-4f7c-8530-882b77261bd9</t>
+  </si>
+  <si>
+    <t>a85724d3-f3d9-43cd-b443-f48a68b648bc</t>
+  </si>
+  <si>
+    <t>0d43247e-59c0-4873-8d10-8a01906ddd4f</t>
+  </si>
+  <si>
+    <t>05039ee6-1c2b-4e19-8c09-49a8740ff77b</t>
+  </si>
+  <si>
+    <t>afe783b3-26da-4f32-b051-4f6e79b470c7</t>
+  </si>
+  <si>
+    <t>1d3325a7-8e6b-4f3d-b3eb-b2484aed3308</t>
+  </si>
+  <si>
+    <t>3a254277-b93b-4357-bf41-598a1e25113d</t>
+  </si>
+  <si>
+    <t>d6c315fa-0d9f-4160-8fb3-de702a291dbe</t>
+  </si>
+  <si>
+    <t>8fca66e5-6bf6-4770-86fc-566ecd542d33</t>
+  </si>
+  <si>
+    <t>f244910c-3ac4-4454-b2d5-df5338260018</t>
+  </si>
+  <si>
+    <t>4108c682-3d53-40c1-aa98-b617803d7315</t>
+  </si>
+  <si>
+    <t>d08cea1f-3e36-4e95-b0e6-6eebe4b52d41</t>
+  </si>
+  <si>
+    <t>0c00b1bd-68fc-4d8f-9c12-5a2c869b15d5</t>
+  </si>
+  <si>
+    <t>56a3c844-3f91-4872-9646-0ece968077e9</t>
+  </si>
+  <si>
+    <t>615e83a8-5c60-4112-afb6-2154d3a7dd77</t>
+  </si>
+  <si>
+    <t>a2aa5a71-4887-464b-9fde-4c73c54e9e4a</t>
+  </si>
+  <si>
+    <t>d32cdfd6-cf64-4989-b747-23ce9228667a</t>
+  </si>
+  <si>
+    <t>a4df48df-1114-4ffa-b1f7-99ea4c2e92bd</t>
+  </si>
+  <si>
+    <t>5089af6b-1158-49de-8186-729aa6222e9c</t>
+  </si>
+  <si>
+    <t>f8b5ee28-d774-4493-8245-e64f169671e5</t>
+  </si>
+  <si>
+    <t>80f0d3d5-0bef-41fc-80af-d7ccfb59a861</t>
+  </si>
+  <si>
+    <t>9a831f4e-5265-4642-a25c-9beaeecffa3f</t>
+  </si>
+  <si>
+    <t>75406243-26ca-4367-95b0-7d5b94859636</t>
+  </si>
+  <si>
+    <t>72251710-abab-4cd9-a4e9-504d1f167b23</t>
+  </si>
+  <si>
+    <t>96df4a9d-d133-49db-be8b-e55a6ee23a35</t>
+  </si>
+  <si>
+    <t>2fb1f44c-0973-4be1-aa3b-70b57629f6bb</t>
+  </si>
+  <si>
+    <t>d49b5786-5652-49a9-82fd-17d6067d964e</t>
+  </si>
+  <si>
+    <t>9cd545fe-d2bf-4de4-b1d6-ab14f624103d</t>
+  </si>
+  <si>
+    <t>62651972-e65e-4ae9-85ef-66af8e098aa9</t>
+  </si>
+  <si>
+    <t>f18e6e1c-f012-4514-92a8-f2e345d90329</t>
+  </si>
+  <si>
+    <t>1366e0bf-6597-48c1-b0c0-832a7aa69d3f</t>
+  </si>
+  <si>
+    <t>4980455b-a4bd-4ad5-b770-de8221ab3388</t>
+  </si>
+  <si>
+    <t>ac88a9da-ab0d-4ab0-be61-5ce4b6f0191e</t>
+  </si>
+  <si>
+    <t>7a584777-ed08-4576-9fcf-dc78e488832e</t>
+  </si>
+  <si>
+    <t>13271e6b-97b6-43ec-9ebb-fdf8443b8362</t>
+  </si>
+  <si>
+    <t>c6f5b3d4-932b-4f14-b321-2695eb5b444b</t>
+  </si>
+  <si>
+    <t>a7b08840-2420-416b-bfa2-bac89863bab8</t>
+  </si>
+  <si>
+    <t>82ea4ecb-402e-4821-b42c-ebdbda8896f6</t>
+  </si>
+  <si>
+    <t>556e38e5-12c2-4443-bd2f-46096616600a</t>
+  </si>
+  <si>
+    <t>c2d970ea-2a23-4cba-bf14-b6d77ec7650c</t>
+  </si>
+  <si>
+    <t>0477cf57-6499-4a76-b3bc-63021b76441e</t>
+  </si>
+  <si>
+    <t>9115d96a-81eb-424f-9c4c-243d753d3a71</t>
+  </si>
+  <si>
+    <t>0e309689-d4ef-4237-af39-1b741473d7f4</t>
+  </si>
+  <si>
+    <t>e6ed95ba-9dd4-48b1-a4eb-5d4880ce5c2e</t>
+  </si>
+  <si>
+    <t>f36f3649-c662-417a-acda-d6797497ac00</t>
+  </si>
+  <si>
+    <t>0d371daa-38a3-4e78-9506-0f9b0b533f10</t>
+  </si>
+  <si>
+    <t>61aeadcf-f223-46b3-8c05-15cdf53b4470</t>
+  </si>
+  <si>
+    <t>f48094a1-8a6c-4222-a4cc-114b13b5ccd7</t>
+  </si>
+  <si>
+    <t>a63d64f9-adcf-4309-9f4c-6ee2ab0adfe4</t>
+  </si>
+  <si>
+    <t>f5174636-a95f-40c3-bf29-fcfcec54c3b3</t>
+  </si>
+  <si>
+    <t>b810fe10-b5c6-402a-91d0-b348d815b06b</t>
+  </si>
+  <si>
+    <t>d9114d65-f674-4c1f-880e-c76df7b1153b</t>
+  </si>
+  <si>
+    <t>386043d3-379b-4bb6-b676-d0d80d9d5a75</t>
+  </si>
+  <si>
+    <t>df27b3b0-3058-47d4-b396-8fe51af09b40</t>
+  </si>
+  <si>
+    <t>61d5878b-16ad-465a-8dc8-c2b29bdb8ef7</t>
+  </si>
+  <si>
+    <t>97ccd6a4-a467-4550-8965-cd0140c06a83</t>
+  </si>
+  <si>
+    <t>484a484c-6843-4e62-bea4-e0c99dc41c5b</t>
+  </si>
+  <si>
+    <t>0d9115b0-a73d-466e-ba4b-5ad21c5a452a</t>
+  </si>
+  <si>
+    <t>ac0ba227-2265-4435-a744-a46c8cd00e16</t>
+  </si>
+  <si>
+    <t>0dfe8f39-7040-4738-a194-f9f2e25b3f48</t>
+  </si>
+  <si>
+    <t>28423d0d-0eeb-4184-b4d0-23e05d08bab6</t>
+  </si>
+  <si>
+    <t>28569574-49e8-4ced-b015-673be37bc18a</t>
+  </si>
+  <si>
+    <t>05e8bf39-f240-434b-aa2f-643765c6b03b</t>
+  </si>
+  <si>
+    <t>0394bc19-bff4-46e7-bb9f-915fa51d42d1</t>
+  </si>
+  <si>
+    <t>6f8661b6-5030-40f3-8f72-cc3eaa8a307f</t>
+  </si>
+  <si>
+    <t>bf197c65-a6f2-4d94-b27e-77d4c02baedd</t>
+  </si>
+  <si>
+    <t>15c84e0d-b04d-4fbd-9151-f87477b6bf94</t>
+  </si>
+  <si>
+    <t>2dbb5e5d-dc34-4e05-997f-d0e853b6fbe4</t>
+  </si>
+  <si>
+    <t>1100534f-da85-4039-b304-120cff6bf9b8</t>
+  </si>
+  <si>
+    <t>34bbe8ce-7b22-4aad-893a-64d843b06616</t>
+  </si>
+  <si>
+    <t>a14e5609-5d90-427c-9803-d0d600342213</t>
+  </si>
+  <si>
+    <t>f2279463-97f0-4496-99ae-00b457735bfa</t>
+  </si>
+  <si>
+    <t>066400fd-1dc0-413d-b36a-e7f45ccc625b</t>
+  </si>
+  <si>
+    <t>bee50522-cb60-4d0c-99fd-7b2f8dc02294</t>
+  </si>
+  <si>
+    <t>20e7d925-eb0e-4976-9a28-3a2accc8b453</t>
+  </si>
+  <si>
+    <t>5448d944-0c84-4246-bd7e-5a865a9cba41</t>
+  </si>
+  <si>
+    <t>2f16c955-f2f4-4be3-8d56-1fe453804f09</t>
+  </si>
+  <si>
+    <t>51788420-1d06-47ed-9d8c-e9d0d1a0c286</t>
+  </si>
+  <si>
+    <t>6460ebd9-d939-4ebd-85c1-27b55b3398b3</t>
+  </si>
+  <si>
+    <t>46bfcce0-d88f-40e9-a436-7c4a3adc74c2</t>
+  </si>
+  <si>
+    <t>aecdc9b7-ea78-4c7f-8bb2-b5d1fd342e2e</t>
+  </si>
+  <si>
+    <t>9403aa4d-a885-401b-83c3-f98f5a9e5984</t>
+  </si>
+  <si>
+    <t>749e0b65-1a32-46c9-a0e8-ab1bc33fed5c</t>
+  </si>
+  <si>
+    <t>bd5c693d-825b-4be1-9fe9-6c494709b4a7</t>
+  </si>
+  <si>
+    <t>af7ce373-77ca-4a21-928b-1b88a7e2257e</t>
+  </si>
+  <si>
+    <t>f014fa44-464f-49c0-8693-d8ca09f1e787</t>
+  </si>
+  <si>
+    <t>3cba3e54-1fa7-40fd-ad13-bdbf74aaa4e0</t>
+  </si>
+  <si>
+    <t>f216f3ff-8254-4aa4-badd-bafa5d36ad86</t>
+  </si>
+  <si>
+    <t>bc4af89b-2724-495d-a4b1-9005727df2f6</t>
+  </si>
+  <si>
+    <t>ede974f3-f278-4bea-b7fc-c9fe5a04a08c</t>
+  </si>
+  <si>
+    <t>256fc914-460a-481b-a8c3-629ba8b83867</t>
+  </si>
+  <si>
+    <t>852d664b-ebdf-4475-9c23-4b1c4d00a028</t>
+  </si>
+  <si>
+    <t>3daa3b67-b6e4-4668-9d79-e7fcf90cf9df</t>
+  </si>
+  <si>
+    <t>7280da74-e89a-41c2-9075-68a1d7587a8b</t>
+  </si>
+  <si>
+    <t>379efd90-b495-4fe7-93aa-04f02d1ccfa0</t>
+  </si>
+  <si>
+    <t>d030a3c2-3506-4287-aab8-c882fc45f0c9</t>
+  </si>
+  <si>
+    <t>65d93ddb-f40b-42aa-956d-3b2651ddd448</t>
+  </si>
+  <si>
+    <t>a63b22d7-5abc-4e3e-90e9-57deef9b0fd0</t>
+  </si>
+  <si>
+    <t>56e9875c-b5db-4245-a31b-85314f34b5a0</t>
+  </si>
+  <si>
+    <t>be020e80-cc4c-4526-80e4-69f1a366d0e9</t>
+  </si>
+  <si>
+    <t>07c39ac1-00ee-4d6e-9eb1-eab53c2e50ad</t>
+  </si>
+  <si>
+    <t>ced2d837-ab48-48f0-8315-0cbe23076aae</t>
+  </si>
+  <si>
+    <t>f8eaf200-d1b0-4cde-b8a0-a24cca4bb8d4</t>
+  </si>
+  <si>
+    <t>f81ed0c8-bd01-4473-b8dd-8ec2e60fc057</t>
+  </si>
+  <si>
+    <t>93855d25-8e7a-4c04-98a4-b85b0f764403</t>
+  </si>
+  <si>
+    <t>c80e58f7-ca78-4e5c-9f47-f27f8672cb40</t>
+  </si>
+  <si>
+    <t>39683105-09b7-4e98-a821-a575a205eece</t>
+  </si>
+  <si>
+    <t>ff9626f6-e2d1-4da8-b4e1-e95b24acaeaf</t>
+  </si>
+  <si>
+    <t>bf6ab902-5e8c-4eea-b24f-95591e99c03a</t>
+  </si>
+  <si>
+    <t>3b3e6413-9d0a-4ce4-9993-c4cd81db5f3e</t>
+  </si>
+  <si>
+    <t>f90e25eb-d983-45ac-a742-7d0d10d0ae4d</t>
+  </si>
+  <si>
+    <t>59b129af-a3ef-42e8-8be8-9168a3b73abc</t>
+  </si>
+  <si>
+    <t>65b0c8d9-7889-408b-b5fb-db4062b4bb1d</t>
+  </si>
+  <si>
+    <t>35dcf27b-8c53-4667-98fc-729e55185e2f</t>
+  </si>
+  <si>
+    <t>ad34aeea-609b-49b7-8740-4a7615775683</t>
+  </si>
+  <si>
+    <t>c3846b16-75ea-4859-be80-f8e7c9ee457e</t>
+  </si>
+  <si>
+    <t>41fc4378-33c5-4730-8163-475a8d28cc21</t>
+  </si>
+  <si>
+    <t>2a1ac4fa-cef0-4a86-8a76-6ea1f342406d</t>
+  </si>
+  <si>
+    <t>4810241b-1a31-4c17-8a65-f7a55191d7aa</t>
+  </si>
+  <si>
+    <t>0761ab26-d64e-411a-9e41-f2792ab780b0</t>
+  </si>
+  <si>
+    <t>2647f87a-a9cd-43b1-9655-9533db7569cf</t>
+  </si>
+  <si>
+    <t>67d93da7-1603-4b4c-ae86-0cc853f9a9a7</t>
+  </si>
+  <si>
+    <t>64e9d4fa-b89d-4ae9-a222-ad4cd4a251d3</t>
+  </si>
+  <si>
+    <t>2476b864-a73f-402e-8398-b018a44efab2</t>
+  </si>
+  <si>
+    <t>f01a4122-9fe9-416d-b74e-12956aca6d45</t>
+  </si>
+  <si>
+    <t>9a13b2b4-f9f4-443f-92e6-7161883e7301</t>
+  </si>
+  <si>
+    <t>17b2f220-d61a-4259-a502-73a35ad2e91d</t>
+  </si>
+  <si>
+    <t>00ba02b3-7f66-48fc-a252-6a5898589a1d</t>
+  </si>
+  <si>
+    <t>b813a94a-aeb0-44aa-acb8-b3bfc0cb9763</t>
+  </si>
+  <si>
+    <t>cdb728df-ee0a-4156-a1cc-11fced7b64da</t>
+  </si>
+  <si>
+    <t>4e68c359-c6c0-4afa-a20f-aec712164464</t>
+  </si>
+  <si>
+    <t>1c31bbfa-3fbe-4c06-908e-c977d0ab180e</t>
+  </si>
+  <si>
+    <t>94ee0341-1bd9-46c2-aea6-f4e1909ecbe5</t>
+  </si>
+  <si>
+    <t>e1ed1e80-b239-4e9f-9b42-0a51f67dfaba</t>
+  </si>
+  <si>
+    <t>170e8f73-cf86-4fde-9d36-327e1f499405</t>
+  </si>
+  <si>
+    <t>cd5dea83-f2d7-49bc-98ce-12e6ce15107d</t>
+  </si>
+  <si>
+    <t>27bb535a-0d5f-4985-9926-7bb87d1528d1</t>
+  </si>
+  <si>
+    <t>36825688-11d9-4f0c-960e-a90fb628c793</t>
+  </si>
+  <si>
+    <t>bb688264-95cd-4b0b-a41d-d3b9a54bab88</t>
+  </si>
+  <si>
+    <t>8c9320f5-a503-4ba8-9c5a-edb3f3baf6ed</t>
+  </si>
+  <si>
+    <t>caaa9716-bcf4-4029-9955-320b952b2e3f</t>
+  </si>
+  <si>
+    <t>1ec8efe0-630c-48e3-aaa1-b76bb6958bf7</t>
+  </si>
+  <si>
+    <t>aa922638-f554-4207-9f5c-9394e1521a33</t>
+  </si>
+  <si>
+    <t>22df213e-02ed-45de-b216-e8ed88533be7</t>
+  </si>
+  <si>
+    <t>c1d32d87-2400-4e1d-9dac-04d38fdfd098</t>
+  </si>
+  <si>
+    <t>ca8b7dca-d442-4aed-99f8-25f2bcc3a20f</t>
+  </si>
+  <si>
+    <t>d5e83f54-69a0-4a5b-9886-5ffa57525b1a</t>
+  </si>
+  <si>
+    <t>24b2dd34-6251-42fc-86d5-39db844ac0cf</t>
+  </si>
+  <si>
+    <t>452e79e9-df9e-41f9-ba60-4bd8bc9fe003</t>
+  </si>
+  <si>
+    <t>2abaf4ac-710c-461a-8ba3-e2971918cd4b</t>
+  </si>
+  <si>
+    <t>a6688871-afbd-450b-97b5-5985a00bdaba</t>
+  </si>
+  <si>
+    <t>2ebd768b-c2ae-4c5c-a897-8972af1bcd23</t>
+  </si>
+  <si>
+    <t>f492f17f-0b26-40fe-985c-980021f3b10d</t>
+  </si>
+  <si>
+    <t>d472db90-ecbd-47b8-b3d6-37fe7b004f2e</t>
+  </si>
+  <si>
+    <t>7be3fe59-ee5f-4d55-9465-15006723aa0c</t>
+  </si>
+  <si>
+    <t>dd748d29-6a6b-43dc-a5ef-69ab88dd4dac</t>
+  </si>
+  <si>
+    <t>69b4bcb2-269a-43be-bc31-67e6c807d5d7</t>
+  </si>
+  <si>
+    <t>eb1f3115-5c09-4891-a744-9563529f8aea</t>
+  </si>
+  <si>
+    <t>229a8c40-dee9-461e-b478-123c7f0f463b</t>
+  </si>
+  <si>
+    <t>1c1ad877-8b19-4ff3-8bf6-e6430817435d</t>
+  </si>
+  <si>
+    <t>5b8b70df-a55a-4136-99c5-2ec2b96cc0cf</t>
+  </si>
+  <si>
+    <t>72e35bc4-92e7-4680-9a33-81e57dd2f0b8</t>
+  </si>
+  <si>
+    <t>8a4b375c-8df2-455b-bd5f-ed57a87458c6</t>
+  </si>
+  <si>
+    <t>5b297a3c-2000-4bc8-b2a8-1f32486a46f3</t>
+  </si>
+  <si>
+    <t>c0cb9304-85fe-43fb-9321-174cc39d0546</t>
+  </si>
+  <si>
+    <t>ad9786da-452e-4c2b-ae5e-4b5f86a9b04d</t>
+  </si>
+  <si>
+    <t>d2743264-c023-4a47-95ee-1ff7efa61eb8</t>
+  </si>
+  <si>
+    <t>5c80526f-7a92-454a-be68-385b1153d76d</t>
+  </si>
+  <si>
+    <t>e2bc2ee6-6272-43a4-83ad-bf16558721b5</t>
+  </si>
+  <si>
+    <t>db30c5f0-2990-40b5-b9f1-7061266ba830</t>
+  </si>
+  <si>
+    <t>225f05e9-79db-431d-93bf-254e53f38e9c</t>
+  </si>
+  <si>
+    <t>e712a151-b773-47a4-a76b-f3ae4e1910fa</t>
+  </si>
+  <si>
+    <t>bd14ac41-bde6-4dfe-b7d3-34f04d159e32</t>
+  </si>
+  <si>
+    <t>2d77dc0b-a62a-4143-9e4b-cdbbfbd346f5</t>
+  </si>
+  <si>
+    <t>4f877299-22c4-4d7a-bf6e-7a8cf3f1bd76</t>
+  </si>
+  <si>
+    <t>92646d6f-d4a1-47cd-a431-fa3abfa6242d</t>
+  </si>
+  <si>
+    <t>eddb11c8-aca4-41b1-8820-e80cb46caf6f</t>
+  </si>
+  <si>
+    <t>cc95fbbd-0acc-48e3-80bc-0d66d01ee69a</t>
+  </si>
+  <si>
+    <t>2925cdc2-c4f3-415b-8aa5-5cfa00ef5559</t>
+  </si>
+  <si>
+    <t>16c48ebf-31ac-4a4c-a06f-026e581759d1</t>
+  </si>
+  <si>
+    <t>4485197c-345a-47cc-9ed0-d963f90cbb55</t>
+  </si>
+  <si>
+    <t>802f298e-bec5-4963-b581-f8564ffd56a1</t>
+  </si>
+  <si>
+    <t>a7321523-1d93-4de2-851f-e145a60c15cb</t>
+  </si>
+  <si>
+    <t>3873687f-b0e7-41eb-9c74-a19d0d4cf00b</t>
+  </si>
+  <si>
+    <t>d70105c7-f33f-4e67-9371-f3cf92e3e430</t>
+  </si>
+  <si>
+    <t>4259db90-3e42-45b4-ba77-8434545950f5</t>
+  </si>
+  <si>
+    <t>7b526ba7-2271-4a8e-922a-9e5416c09e1b</t>
+  </si>
+  <si>
+    <t>b13e6a5f-f69b-451b-bd59-d77fde32a1f0</t>
+  </si>
+  <si>
+    <t>2b03c114-58ea-4f95-bc23-7505cd9fa263</t>
+  </si>
+  <si>
+    <t>22fc3d82-c412-4cda-b854-4ae220280c20</t>
+  </si>
+  <si>
+    <t>ed31aa8d-d395-43b8-953e-6ff89daa149d</t>
+  </si>
+  <si>
+    <t>7fde26e1-529c-4430-adc5-b450df4c9f17</t>
+  </si>
+  <si>
+    <t>13fba698-e5b0-47ba-a697-44fa32654e93</t>
+  </si>
+  <si>
+    <t>444b9125-010a-4168-a8d3-a2c68593cd42</t>
+  </si>
+  <si>
+    <t>00dda9cc-b74d-4be3-9af2-8026f41e28f4</t>
+  </si>
+  <si>
+    <t>d261d886-6fd2-4a53-9714-1904303d27d2</t>
+  </si>
+  <si>
+    <t>7fd2ef38-f456-4c4c-bba0-93d1457df7d4</t>
+  </si>
+  <si>
+    <t>cbdfe715-c10d-44f2-a5e1-71be7bf252ed</t>
+  </si>
+  <si>
+    <t>7d21e826-3b6a-424f-801f-018a5c84ef5e</t>
+  </si>
+  <si>
+    <t>df63e38c-2559-40ad-9ee5-c01b55a3a9f0</t>
+  </si>
+  <si>
+    <t>ceab18d7-a0f3-4fef-b6e8-df239391f350</t>
+  </si>
+  <si>
+    <t>ebcb42da-b6a5-440a-8e24-5ae4cb2b6eb6</t>
+  </si>
+  <si>
+    <t>9b3088ae-7591-4158-943b-2146a2be5827</t>
+  </si>
+  <si>
+    <t>ed0a1d63-8889-42f8-bc9a-6e54bf275bc9</t>
+  </si>
+  <si>
+    <t>84ce9b05-64c5-4890-bc24-4ae6217c99b7</t>
+  </si>
+  <si>
+    <t>ff38f193-4df2-4c32-b218-88285510cb45</t>
+  </si>
+  <si>
+    <t>42bfc590-a81a-4b33-9fd7-594fd86d02cc</t>
+  </si>
+  <si>
+    <t>d65f895f-e687-43f5-a5af-aae1734cf075</t>
+  </si>
+  <si>
+    <t>c62f0923-46ff-495e-b3fe-2b5efb638b10</t>
+  </si>
+  <si>
+    <t>3e93871f-324e-4e9d-8187-8d5b7b95251e</t>
+  </si>
+  <si>
+    <t>09359dfd-fd24-44a9-b765-ad37ec8e5ccf</t>
+  </si>
+  <si>
+    <t>109b11f5-7eb2-48e3-b122-9bf03c0b9faf</t>
+  </si>
+  <si>
+    <t>e2135614-6964-496b-aadb-9a5cfdc19aad</t>
+  </si>
+  <si>
+    <t>0e75e1e4-a6b7-4e7f-b603-b79a21e864cd</t>
+  </si>
+  <si>
+    <t>26dc9bee-4fe4-4085-b5b7-c4beb69d4e9d</t>
+  </si>
+  <si>
+    <t>59a331e3-c02c-4992-9b92-ce002fd27848</t>
+  </si>
+  <si>
+    <t>2594d278-fcec-4a70-a78d-8abaf72c92a6</t>
+  </si>
+  <si>
+    <t>190a8b13-e851-4004-8f3f-3b76f6015766</t>
+  </si>
+  <si>
+    <t>3ca290b1-5ad0-419c-a4a9-cc34ef5f83e6</t>
+  </si>
+  <si>
+    <t>9e74b124-726a-4cb2-b984-776dd4f02162</t>
+  </si>
+  <si>
+    <t>0298ccab-f8e3-499f-a60f-7fc8cd48310a</t>
+  </si>
+  <si>
+    <t>b3f68e07-d804-46c8-9e80-dba252d3dbc5</t>
+  </si>
+  <si>
+    <t>a43cde0b-1702-4c29-b4f6-854e3be6f0e3</t>
+  </si>
+  <si>
+    <t>bc0b62f0-082e-4006-9405-795280d9f13e</t>
+  </si>
+  <si>
+    <t>8de24694-f6d1-4adf-9d71-5b2fc0783836</t>
+  </si>
+  <si>
+    <t>47f0d8ba-6011-47d6-8fac-970af799f7a0</t>
+  </si>
+  <si>
+    <t>124b7ab5-8c5e-47ed-a492-7531b181f555</t>
+  </si>
+  <si>
+    <t>110c87f2-ebc5-48a1-8f9f-7502de371811</t>
+  </si>
+  <si>
+    <t>ce8ee2c8-7ae2-495c-8e3b-31479bc54da3</t>
+  </si>
+  <si>
+    <t>a8f61ebb-7599-4969-b1e2-f74a57f467f2</t>
+  </si>
+  <si>
+    <t>cfdf2320-634d-4987-ae4c-4f1b55be4f4d</t>
+  </si>
+  <si>
+    <t>a7205a8b-2412-45dd-abb8-4f452378d8a5</t>
+  </si>
+  <si>
+    <t>2b0d6aed-899d-46b8-b75b-5031d55c98b5</t>
+  </si>
+  <si>
+    <t>6976ab3c-ae80-4e24-9489-5c85e1a649e7</t>
+  </si>
+  <si>
+    <t>6eed66a1-0887-4b7c-b019-8846c257bb4e</t>
+  </si>
+  <si>
+    <t>ca25fb84-f3d2-4791-8bd3-00008e0c020c</t>
+  </si>
+  <si>
+    <t>2571653f-3a51-43e2-9574-9788c8806d2e</t>
+  </si>
+  <si>
+    <t>6f95e191-c06c-4566-af52-0eac40bdcac2</t>
+  </si>
+  <si>
+    <t>db1f74a9-49d8-4128-9558-938d475e9ba9</t>
+  </si>
+  <si>
+    <t>1203b581-4a62-47ce-89b5-9c639d711641</t>
+  </si>
+  <si>
+    <t>c1fed596-0244-4406-86bd-cf84bb5bb2e5</t>
+  </si>
+  <si>
+    <t>19b8b0d0-ce7d-4088-9619-2c6b067a0d52</t>
+  </si>
+  <si>
+    <t>4a4763c6-3921-4de5-a4ea-868232f692b5</t>
+  </si>
+  <si>
+    <t>40e862d5-577c-47ce-8c44-7eb82a394aae</t>
+  </si>
+  <si>
+    <t>7edc0917-3126-4aea-b287-40f3fdcc5dd3</t>
+  </si>
+  <si>
+    <t>0a9686a9-ed1b-4ee6-b276-f37812470d31</t>
+  </si>
+  <si>
+    <t>047e1906-7465-4a88-a7c9-28b5b03cf657</t>
+  </si>
+  <si>
+    <t>fc630f4c-1b5b-4725-b498-463e68293903</t>
+  </si>
+  <si>
+    <t>dc782382-b3d4-4df9-8c1c-b72d79537662</t>
+  </si>
+  <si>
+    <t>7eb479cb-9d81-48df-84a6-26be76518ec8</t>
+  </si>
+  <si>
+    <t>c7b0e592-f95c-4cb3-8ea3-81e6a4a761e9</t>
+  </si>
+  <si>
+    <t>a1938333-a655-4664-97a1-4a993aeae070</t>
+  </si>
+  <si>
+    <t>da76d8d5-f7e6-4f53-aa42-76fa46a33bac</t>
+  </si>
+  <si>
+    <t>44ff2df5-693e-409a-9d4c-4fc1e9b2f24a</t>
+  </si>
+  <si>
+    <t>1c501c45-be02-4103-bf45-e441f853c45b</t>
+  </si>
+  <si>
+    <t>cdd7ab2b-390a-4490-b42e-f4d1c952a951</t>
+  </si>
+  <si>
+    <t>f9b306dd-8239-469b-90cd-210e7e04e400</t>
+  </si>
+  <si>
+    <t>b82a5ffd-1f1e-4de4-9299-05ebf8b5c617</t>
+  </si>
+  <si>
+    <t>77033baf-2068-4f78-bc24-e35a4ce61fa3</t>
+  </si>
+  <si>
+    <t>f8f5b38b-454b-4e3e-a1a3-441ba44afcf3</t>
+  </si>
+  <si>
+    <t>9d077c79-9870-4abf-a476-9a3dfd895f22</t>
+  </si>
+  <si>
+    <t>96a7d83c-b06e-4042-aaf5-3c7e01f9e4f9</t>
+  </si>
+  <si>
+    <t>7fce97b2-d406-4576-991b-bb6de226b8d0</t>
+  </si>
+  <si>
+    <t>104281e3-73b8-43e1-8e46-9bbf4f98fb24</t>
+  </si>
+  <si>
+    <t>17141a77-9aa9-4ab8-b434-e8dc18ba248f</t>
+  </si>
+  <si>
+    <t>30830fd8-ff45-4ab9-b117-45e60678d92f</t>
+  </si>
+  <si>
+    <t>e84dec5b-f297-4832-9e33-ece7baafedcd</t>
+  </si>
+  <si>
+    <t>ea459dde-5306-4b18-b649-bd1ec3f660da</t>
+  </si>
+  <si>
+    <t>a73bd487-b4a0-4db6-8b68-9a5144e6ee0b</t>
+  </si>
+  <si>
+    <t>400f1034-46d1-4d89-816a-b8df1ca816a6</t>
+  </si>
+  <si>
+    <t>bb8e2862-0edf-4386-8870-eff80aae873a</t>
+  </si>
+  <si>
+    <t>9fb5af93-7c34-4609-8fa8-cf90a6ab9d00</t>
+  </si>
+  <si>
+    <t>2f47270d-149b-4256-a812-ab369b2d09ee</t>
+  </si>
+  <si>
+    <t>9e2a0f84-27f7-4fc4-988f-0393ca1415a3</t>
+  </si>
+  <si>
+    <t>6d35d21c-b8b8-48a2-9d13-1b7c73a0e74a</t>
+  </si>
+  <si>
+    <t>cbd4976d-bca3-4225-862a-f6c3e18c3579</t>
+  </si>
+  <si>
+    <t>60aaef46-970a-4402-aadc-06c4b732570a</t>
+  </si>
+  <si>
+    <t>c7dec6af-ac15-4aa8-a002-bb2bef802e65</t>
+  </si>
+  <si>
+    <t>6cdad34b-e158-43c4-9f1e-0f50c8fb0e72</t>
+  </si>
+  <si>
+    <t>fa92904c-026e-45ef-942b-84de1caf1252</t>
+  </si>
+  <si>
+    <t>caedf881-2e52-409a-af8b-ab53c806700c</t>
+  </si>
+  <si>
+    <t>c9feae6b-1bcb-4045-b117-056c095011e4</t>
+  </si>
+  <si>
+    <t>32416645-e12f-47c7-b513-f50ffd642f9c</t>
+  </si>
+  <si>
+    <t>178e5e63-8b95-4156-9279-fd0408c64224</t>
+  </si>
+  <si>
+    <t>08f8b494-072f-47db-9b88-51dffff579d9</t>
+  </si>
+  <si>
+    <t>37802718-2a75-488f-b862-1080adbd4b54</t>
+  </si>
+  <si>
+    <t>a9334fbd-d59a-4032-b8b2-ed14f004f223</t>
+  </si>
+  <si>
+    <t>9ad609fe-de8d-49c2-ad25-dbabe724ffaf</t>
+  </si>
+  <si>
+    <t>21e3588d-f6e7-4d45-9ce4-8f5ba8fdcfd2</t>
+  </si>
+  <si>
+    <t>f3b16c44-fe11-4778-8d57-a16d44a71e2a</t>
+  </si>
+  <si>
+    <t>877d305f-500a-4dcd-a324-b0e7d1cb129e</t>
+  </si>
+  <si>
+    <t>6ffb7e16-5492-4257-81df-ef8667723237</t>
+  </si>
+  <si>
+    <t>8964a156-149c-460a-8268-b3e58fbae590</t>
+  </si>
+  <si>
+    <t>9951b446-6a17-4351-a10c-57c85979796a</t>
+  </si>
+  <si>
+    <t>323111f3-0410-4564-9a19-cd66321e9dc3</t>
+  </si>
+  <si>
+    <t>f36bb176-4f0b-411f-99a7-2b9b7df4091e</t>
+  </si>
+  <si>
+    <t>31400250-6926-4d33-a0f0-4b356127f0aa</t>
+  </si>
+  <si>
+    <t>a3a4d024-5814-41f0-9ede-17402f75c16e</t>
+  </si>
+  <si>
+    <t>bffff469-8d6a-4880-b78a-aabd79434ad4</t>
+  </si>
+  <si>
+    <t>20a2c753-11d9-4338-bed8-abf56a50d8ea</t>
+  </si>
+  <si>
+    <t>630a59de-5ffe-46ec-addc-777778d1d5bc</t>
+  </si>
+  <si>
+    <t>ad0900b3-b083-45d7-812f-232a4104a21e</t>
+  </si>
+  <si>
+    <t>18a6c7ab-cf1d-45a9-a461-38951f104e70</t>
+  </si>
+  <si>
+    <t>035478cc-b987-4fc0-a850-556ce929ce78</t>
+  </si>
+  <si>
+    <t>be0608ce-bfce-4655-ad26-0591d1c0edb7</t>
+  </si>
+  <si>
+    <t>0a63a1ea-cbf5-41b6-87e1-4e70369fe2ce</t>
+  </si>
+  <si>
+    <t>8c17b9f4-cf40-43f9-b72b-152f0725cf79</t>
+  </si>
+  <si>
+    <t>4755a7ae-84b1-44f6-92dc-d45fe655334e</t>
+  </si>
+  <si>
+    <t>466432a5-d015-46cf-b062-b491055e6ef5</t>
+  </si>
+  <si>
+    <t>45e0cd18-9ec2-4a99-9255-8aa3f5938310</t>
+  </si>
+  <si>
+    <t>5b9a78de-a698-49bb-a2ba-830878f70c5f</t>
+  </si>
+  <si>
+    <t>aa2c8064-6f80-404a-b734-0a496d5021fe</t>
+  </si>
+  <si>
+    <t>a4c7657a-22c5-40b9-a040-0fcbb6627515</t>
+  </si>
+  <si>
+    <t>c3283923-ba01-4ce8-8625-3244a5273564</t>
+  </si>
+  <si>
+    <t>326f8da1-2f12-4d5c-8401-66ba552e86dc</t>
+  </si>
+  <si>
+    <t>b16ea222-6fda-4ea8-b09e-e7cb4b4957a7</t>
+  </si>
+  <si>
+    <t>d1a283ff-7075-447e-a206-4e19c7fac589</t>
+  </si>
+  <si>
+    <t>751d8462-fa4c-471c-827b-4a702cdc4f3b</t>
+  </si>
+  <si>
+    <t>1a1fc05a-1651-45b7-a36f-e003e98fbed6</t>
+  </si>
+  <si>
+    <t>4de0f7f3-0b0f-45f3-a5b3-4ef679713781</t>
+  </si>
+  <si>
+    <t>43b0108c-f14d-4005-9c3d-fd5a2a5d70d2</t>
+  </si>
+  <si>
+    <t>2d675920-5119-4cf8-95fc-3fe3f7a514ad</t>
+  </si>
+  <si>
+    <t>1eec3106-4952-4be1-b215-b30026c30647</t>
+  </si>
+  <si>
+    <t>d9dbef42-bd80-4a79-a749-f1a9009f9ba3</t>
+  </si>
+  <si>
+    <t>cdf62173-75cc-4a80-9503-821602bc224f</t>
+  </si>
+  <si>
+    <t>bef423e0-5aa8-47f0-b143-0042b15954bc</t>
+  </si>
+  <si>
+    <t>48c3b06d-cbfa-49f4-8104-98d809d4baed</t>
+  </si>
+  <si>
+    <t>f2c25422-1ac6-46a9-9ef1-6b6e08289c9c</t>
+  </si>
+  <si>
+    <t>ac24c463-137c-43a2-b491-64f19bb9f98f</t>
+  </si>
+  <si>
+    <t>193b727d-6e79-4d64-8160-a07c0ec6173d</t>
+  </si>
+  <si>
+    <t>66d2775a-c3c6-41d0-9ec5-f3ad8c3171c0</t>
+  </si>
+  <si>
+    <t>c484e5eb-a8a5-4872-ae0a-c00568734153</t>
+  </si>
+  <si>
+    <t>dfb34662-cc9f-437e-b60e-7d66f545d5e7</t>
+  </si>
+  <si>
+    <t>dac00514-c370-4463-b095-37d2106ff60b</t>
+  </si>
+  <si>
+    <t>5e4e7cbf-0f69-4843-8c58-95fdc83fb470</t>
+  </si>
+  <si>
+    <t>4fca153d-119a-4769-9f59-efb41089aefc</t>
+  </si>
+  <si>
+    <t>cfee7538-58b1-457c-b742-94b7dbd5ce09</t>
+  </si>
+  <si>
+    <t>ad86ad1c-5ad0-4730-900f-46255f10062f</t>
+  </si>
+  <si>
+    <t>5ebc086d-24c5-42d1-8bc2-d0c7a872d889</t>
+  </si>
+  <si>
+    <t>8b90128e-2ca8-42f4-9baf-ee4c86594ee9</t>
+  </si>
+  <si>
+    <t>e5af7b8b-8d93-4cd2-8cf9-92220909dadc</t>
+  </si>
+  <si>
+    <t>0dc66570-3ed6-435b-8047-cca3bcb3a7dd</t>
+  </si>
+  <si>
+    <t>131aa5a0-b73c-42c4-8216-1591bf78003f</t>
+  </si>
+  <si>
+    <t>131a8281-825a-4c32-8745-f44cc45d9ee3</t>
+  </si>
+  <si>
+    <t>bc026f13-a32c-46b0-896a-c7190be8510d</t>
+  </si>
+  <si>
+    <t>351cf153-f1b1-40dc-b815-7737514da765</t>
+  </si>
+  <si>
+    <t>1c301312-f68c-4a65-9398-f9e0f569533a</t>
+  </si>
+  <si>
+    <t>5d795434-a4bb-4e6b-8648-e8b8a64ff910</t>
+  </si>
+  <si>
+    <t>a4310bdd-0bdf-4bee-8f9f-ca7cc7137ecf</t>
+  </si>
+  <si>
+    <t>bc018d93-2a9a-460a-af25-7b8aa19b26f8</t>
+  </si>
+  <si>
+    <t>be581463-de77-476b-9d8a-df305d4336f8</t>
+  </si>
+  <si>
+    <t>df80ebe5-9b90-462b-be89-2f07e5a8d4aa</t>
+  </si>
+  <si>
+    <t>3b2463ee-24dd-42d7-a81f-48e21b84d774</t>
+  </si>
+  <si>
+    <t>e1a0dbff-8d5b-429a-8e21-ff5f6a1aa5ca</t>
+  </si>
+  <si>
+    <t>65061c46-4542-4047-a764-c51d66a9df25</t>
+  </si>
+  <si>
+    <t>0c02d348-b698-45ed-b2f0-ff8a17f31a57</t>
+  </si>
+  <si>
+    <t>1e79e36b-39bc-4429-916b-b3c005828157</t>
+  </si>
+  <si>
+    <t>222e6b10-fef6-43ac-931e-93308f2ba189</t>
+  </si>
+  <si>
+    <t>7ed86589-11ec-4cbf-94dd-430d031e1739</t>
+  </si>
+  <si>
+    <t>617e9607-50e7-4793-bab7-14a6614ed62f</t>
+  </si>
+  <si>
+    <t>c1d84020-f811-4aca-ae14-dad1b9ac9b7c</t>
+  </si>
+  <si>
+    <t>c264ff32-eddb-4c1c-b312-4e61a632785c</t>
+  </si>
+  <si>
+    <t>b510bee5-1357-4e41-8cd7-5284df23bd22</t>
+  </si>
+  <si>
+    <t>25133d7a-d26f-4c16-90f1-470089511285</t>
+  </si>
+  <si>
+    <t>7eca1d7c-f347-49d1-bb8f-6155ddb64e99</t>
+  </si>
+  <si>
+    <t>ada5328d-0830-4dcc-8566-8a52933a944c</t>
+  </si>
+  <si>
+    <t>599359d9-1b94-47fa-acd0-8832074849b5</t>
+  </si>
+  <si>
+    <t>2dee2161-3ba2-4a6a-b229-e5f5bebaf0a0</t>
+  </si>
+  <si>
+    <t>ed79a94c-c41e-4d51-85ec-c91b55cff0d6</t>
+  </si>
+  <si>
+    <t>bf06acb4-b334-41b4-9830-e5c0d26ef7db</t>
+  </si>
+  <si>
+    <t>b03a36cb-de29-4a16-8c9e-fd5773e66c46</t>
+  </si>
+  <si>
+    <t>ede831bc-c293-4cac-8f3f-05f5c2e242bc</t>
+  </si>
+  <si>
+    <t>a70c573d-1681-4a27-9d27-2d5770b8148f</t>
+  </si>
+  <si>
+    <t>90f1ca9a-5014-48e7-9b63-01b859f9ec1d</t>
+  </si>
+  <si>
+    <t>757ab6e3-e0e6-4d3a-9117-29725fe4ee45</t>
+  </si>
+  <si>
+    <t>3102402d-78e2-4c1c-8ac7-a58a793a7be4</t>
+  </si>
+  <si>
+    <t>303be9c9-4058-433a-a4ea-a12ca5aaf05a</t>
+  </si>
+  <si>
+    <t>c256e003-c90d-4e98-ae9a-2737f99378c0</t>
+  </si>
+  <si>
+    <t>7736f729-cda8-4076-a454-b629ab7729f6</t>
+  </si>
+  <si>
+    <t>1d1c492d-1202-4387-a972-eea0472ef5e0</t>
+  </si>
+  <si>
+    <t>7fc53743-d27b-4267-8655-ac0df948ca0a</t>
+  </si>
+  <si>
+    <t>679adaf1-ad6f-4555-85fd-fe68d4656de0</t>
+  </si>
+  <si>
+    <t>a70c6c89-bd89-4bcc-9fa8-4c64a395be62</t>
+  </si>
+  <si>
+    <t>5f031783-b4ce-4f91-aaaf-9fa80ebc8cd7</t>
+  </si>
+  <si>
+    <t>d1d8ccb9-2631-4ac3-9d25-d4d1dd41ea9a</t>
+  </si>
+  <si>
+    <t>f8ceb63c-bc09-4ec1-8e7c-0ccce9f92485</t>
+  </si>
+  <si>
+    <t>d09cc870-9dfe-406f-9d8f-d591c34565dc</t>
+  </si>
+  <si>
+    <t>8e39c029-ccea-4ee5-9feb-298c8a10ad9a</t>
+  </si>
+  <si>
+    <t>788f225e-d799-4aad-8042-ab1ea95f7b67</t>
+  </si>
+  <si>
+    <t>c48e4a16-7d8b-492e-b502-ecb005893fb9</t>
+  </si>
+  <si>
+    <t>331c2b0f-c099-45ec-8a9d-127a5cef1feb</t>
+  </si>
+  <si>
+    <t>1a3a8e06-fbae-40ef-95bb-8fd6b0dcc84e</t>
+  </si>
+  <si>
+    <t>0f6f27a1-0eb6-4c85-859d-185823757c06</t>
+  </si>
+  <si>
+    <t>72ba2fda-b00f-43f1-92ad-b6374772d08d</t>
+  </si>
+  <si>
+    <t>27e914de-7bec-42df-9ceb-1be0097e5035</t>
+  </si>
+  <si>
+    <t>7b927f4c-51dd-447c-939f-58430ff45803</t>
+  </si>
+  <si>
+    <t>4e3795db-7131-4448-8262-22a963c3effb</t>
+  </si>
+  <si>
+    <t>18ebe39c-cb63-4f74-87ae-77365ea8e2b1</t>
+  </si>
+  <si>
+    <t>36fce3d9-408f-41bd-842c-cc6afaefad3a</t>
+  </si>
+  <si>
+    <t>45620768-5ebb-42de-8f20-c4404092d274</t>
+  </si>
+  <si>
+    <t>20937843-fac0-4b4e-999a-7bf771d8a744</t>
+  </si>
+  <si>
+    <t>fd378a66-a796-46b3-93f4-81e9a7a16967</t>
+  </si>
+  <si>
+    <t>89b0d0eb-62af-48a9-9079-7b3195aa4164</t>
+  </si>
+  <si>
+    <t>17912e74-264c-4314-a84d-2eb132faab1b</t>
+  </si>
+  <si>
+    <t>49bd41b4-c8b1-4718-90ff-9d38063984f8</t>
+  </si>
+  <si>
+    <t>b2b83e69-7842-403f-8aa4-5376c45c15c2</t>
+  </si>
+  <si>
+    <t>f29c02e5-bc07-415b-9a18-a19282023f29</t>
+  </si>
+  <si>
+    <t>f38c9f06-3fe8-4d28-a736-7e41c1082a86</t>
+  </si>
+  <si>
+    <t>fda29f49-c4b4-4273-b607-89a4d56e7bd1</t>
+  </si>
+  <si>
+    <t>2062f879-327c-48d7-aa41-4b0c0e1d983f</t>
+  </si>
+  <si>
+    <t>01faa3cd-6959-4aae-8641-3a6372c47a71</t>
+  </si>
+  <si>
+    <t>c0c33ae6-fcf7-4f69-a0e7-23b4d5902dae</t>
+  </si>
+  <si>
+    <t>a9113f00-6ca5-444e-832b-4993c9b52b97</t>
+  </si>
+  <si>
+    <t>8b4e256a-1487-4314-835b-408b8b310711</t>
+  </si>
+  <si>
+    <t>248786bc-8c90-4fc5-abb9-4544521b4195</t>
+  </si>
+  <si>
+    <t>90945f3f-2fbd-4725-ae32-235e5d681e10</t>
+  </si>
+  <si>
+    <t>a99172dc-fe1b-42cf-9d8c-49ddc36bec86</t>
+  </si>
+  <si>
+    <t>c91427ec-a335-4359-9394-b3f4a503c2f4</t>
+  </si>
+  <si>
+    <t>57d5f744-6776-4914-859f-985a82eb1314</t>
+  </si>
+  <si>
+    <t>50958680-a5b7-45b1-b7ef-9486658e38cf</t>
+  </si>
+  <si>
+    <t>2492b361-64cd-4e16-bd66-8e6507db507a</t>
+  </si>
+  <si>
+    <t>7a6927dd-1cb3-4abc-8d4d-1446ea1e3967</t>
+  </si>
+  <si>
+    <t>966ca256-8cd8-4078-8751-36fcbdc3381a</t>
+  </si>
+  <si>
+    <t>90fb09df-508d-4c9c-afce-df504abbd757</t>
+  </si>
+  <si>
+    <t>e03cf179-d849-4f29-ac15-c70ca6920a43</t>
+  </si>
+  <si>
+    <t>03f3c131-2875-40fd-bb22-46fa59b88d53</t>
   </si>
   <si>
     <t>Pending</t>

</xml_diff>